<commit_message>
Changing Sql table Structure
</commit_message>
<xml_diff>
--- a/FullStackProject/documentation/serverAPIs.xlsx
+++ b/FullStackProject/documentation/serverAPIs.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Html_CSS\FullStackProject\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F138636A-8B45-444A-8482-B9E77AB3FF49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{771F01A2-CC72-46EC-983F-73C8648F9D46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="16305" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Notes" sheetId="17" r:id="rId1"/>
-    <sheet name="Status" sheetId="15" r:id="rId2"/>
+    <sheet name="Error Code" sheetId="17" r:id="rId1"/>
+    <sheet name="Status Code" sheetId="15" r:id="rId2"/>
     <sheet name="Codes" sheetId="18" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="81">
   <si>
     <t xml:space="preserve">Sr </t>
   </si>
@@ -280,7 +280,7 @@
     <t>Not Implemented</t>
   </si>
   <si>
-    <t>res</t>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -369,7 +369,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -407,11 +407,94 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="14">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -750,7 +833,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D63068D-D3BE-48A3-9140-D51DFAAE2583}">
   <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView topLeftCell="B16" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
@@ -1153,10 +1236,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C18:C25">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
       <formula>"N"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
       <formula>"D"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1166,39 +1249,2317 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8787874B-90D5-45F1-9880-0373B280E830}">
-  <dimension ref="B1:E8"/>
+  <dimension ref="A1:R52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12" style="1"/>
-    <col min="2" max="2" width="23.28515625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="12" style="5"/>
-    <col min="4" max="4" width="12" style="4"/>
-    <col min="5" max="16384" width="12" style="1"/>
+    <col min="1" max="1" width="8.28515625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="13" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="1.42578125" style="11" customWidth="1"/>
+    <col min="4" max="4" width="7.42578125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="12" style="4"/>
+    <col min="6" max="6" width="1.42578125" style="11" customWidth="1"/>
+    <col min="7" max="8" width="12" style="4"/>
+    <col min="9" max="9" width="1.42578125" style="11" customWidth="1"/>
+    <col min="10" max="11" width="12" style="4"/>
+    <col min="12" max="12" width="1.42578125" style="11" customWidth="1"/>
+    <col min="13" max="14" width="12" style="4"/>
+    <col min="15" max="15" width="1.42578125" style="11" customWidth="1"/>
+    <col min="16" max="17" width="12" style="4"/>
+    <col min="18" max="18" width="1.42578125" style="11" customWidth="1"/>
+    <col min="19" max="16384" width="12" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B1" s="4" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="6" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E6" s="6"/>
-    </row>
-    <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E8" s="6"/>
+      <c r="B1" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="N1" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q1" s="13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>0</v>
+      </c>
+      <c r="B2" s="5" t="str">
+        <f>TEXT(DEC2HEX(A2, 5), "00000")</f>
+        <v>00000</v>
+      </c>
+      <c r="D2" s="4">
+        <v>51</v>
+      </c>
+      <c r="E2" s="4" t="str">
+        <f>TEXT(DEC2HEX(D2, 5), "00000")</f>
+        <v>00033</v>
+      </c>
+      <c r="G2" s="4">
+        <v>101</v>
+      </c>
+      <c r="H2" s="4" t="str">
+        <f>TEXT(DEC2HEX(G2, 5), "00000")</f>
+        <v>00065</v>
+      </c>
+      <c r="J2" s="4">
+        <v>151</v>
+      </c>
+      <c r="K2" s="4" t="str">
+        <f>TEXT(DEC2HEX(J2, 5), "00000")</f>
+        <v>00097</v>
+      </c>
+      <c r="M2" s="4">
+        <v>201</v>
+      </c>
+      <c r="N2" s="4" t="str">
+        <f>TEXT(DEC2HEX(M2, 5), "00000")</f>
+        <v>000C9</v>
+      </c>
+      <c r="P2" s="4">
+        <v>251</v>
+      </c>
+      <c r="Q2" s="4" t="str">
+        <f>TEXT(DEC2HEX(P2, 5), "00000")</f>
+        <v>000FB</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5" t="str">
+        <f t="shared" ref="B3:B59" si="0">TEXT(DEC2HEX(A3, 5), "00000")</f>
+        <v>00001</v>
+      </c>
+      <c r="D3" s="4">
+        <v>52</v>
+      </c>
+      <c r="E3" s="4" t="str">
+        <f>TEXT(DEC2HEX(D3, 5), "00000")</f>
+        <v>00034</v>
+      </c>
+      <c r="G3" s="4">
+        <v>102</v>
+      </c>
+      <c r="H3" s="4" t="str">
+        <f>TEXT(DEC2HEX(G3, 5), "00000")</f>
+        <v>00066</v>
+      </c>
+      <c r="J3" s="4">
+        <v>152</v>
+      </c>
+      <c r="K3" s="4" t="str">
+        <f>TEXT(DEC2HEX(J3, 5), "00000")</f>
+        <v>00098</v>
+      </c>
+      <c r="M3" s="4">
+        <v>202</v>
+      </c>
+      <c r="N3" s="4" t="str">
+        <f>TEXT(DEC2HEX(M3, 5), "00000")</f>
+        <v>000CA</v>
+      </c>
+      <c r="P3" s="4">
+        <v>252</v>
+      </c>
+      <c r="Q3" s="4" t="str">
+        <f>TEXT(DEC2HEX(P3, 5), "00000")</f>
+        <v>000FC</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>00002</v>
+      </c>
+      <c r="D4" s="4">
+        <v>53</v>
+      </c>
+      <c r="E4" s="4" t="str">
+        <f t="shared" ref="E4:E52" si="1">TEXT(DEC2HEX(D4, 5), "00000")</f>
+        <v>00035</v>
+      </c>
+      <c r="G4" s="4">
+        <v>103</v>
+      </c>
+      <c r="H4" s="4" t="str">
+        <f t="shared" ref="H4:H30" si="2">TEXT(DEC2HEX(G4, 5), "00000")</f>
+        <v>00067</v>
+      </c>
+      <c r="J4" s="4">
+        <v>153</v>
+      </c>
+      <c r="K4" s="4" t="str">
+        <f t="shared" ref="K4:K30" si="3">TEXT(DEC2HEX(J4, 5), "00000")</f>
+        <v>00099</v>
+      </c>
+      <c r="M4" s="4">
+        <v>203</v>
+      </c>
+      <c r="N4" s="4" t="str">
+        <f t="shared" ref="N4:N30" si="4">TEXT(DEC2HEX(M4, 5), "00000")</f>
+        <v>000CB</v>
+      </c>
+      <c r="P4" s="4">
+        <v>253</v>
+      </c>
+      <c r="Q4" s="4" t="str">
+        <f t="shared" ref="Q4:Q30" si="5">TEXT(DEC2HEX(P4, 5), "00000")</f>
+        <v>000FD</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>00003</v>
+      </c>
+      <c r="D5" s="4">
+        <v>54</v>
+      </c>
+      <c r="E5" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>00036</v>
+      </c>
+      <c r="G5" s="4">
+        <v>104</v>
+      </c>
+      <c r="H5" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>00068</v>
+      </c>
+      <c r="J5" s="4">
+        <v>154</v>
+      </c>
+      <c r="K5" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>0009A</v>
+      </c>
+      <c r="M5" s="4">
+        <v>204</v>
+      </c>
+      <c r="N5" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>000CC</v>
+      </c>
+      <c r="P5" s="4">
+        <v>254</v>
+      </c>
+      <c r="Q5" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>000FE</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>4</v>
+      </c>
+      <c r="B6" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>00004</v>
+      </c>
+      <c r="D6" s="4">
+        <v>55</v>
+      </c>
+      <c r="E6" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>00037</v>
+      </c>
+      <c r="G6" s="4">
+        <v>105</v>
+      </c>
+      <c r="H6" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>00069</v>
+      </c>
+      <c r="J6" s="4">
+        <v>155</v>
+      </c>
+      <c r="K6" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>0009B</v>
+      </c>
+      <c r="M6" s="4">
+        <v>205</v>
+      </c>
+      <c r="N6" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>000CD</v>
+      </c>
+      <c r="P6" s="4">
+        <v>255</v>
+      </c>
+      <c r="Q6" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>000FF</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>5</v>
+      </c>
+      <c r="B7" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>00005</v>
+      </c>
+      <c r="D7" s="4">
+        <v>56</v>
+      </c>
+      <c r="E7" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>00038</v>
+      </c>
+      <c r="G7" s="4">
+        <v>106</v>
+      </c>
+      <c r="H7" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>0006A</v>
+      </c>
+      <c r="J7" s="4">
+        <v>156</v>
+      </c>
+      <c r="K7" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>0009C</v>
+      </c>
+      <c r="M7" s="4">
+        <v>206</v>
+      </c>
+      <c r="N7" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>000CE</v>
+      </c>
+      <c r="P7" s="4">
+        <v>256</v>
+      </c>
+      <c r="Q7" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>00100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>6</v>
+      </c>
+      <c r="B8" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>00006</v>
+      </c>
+      <c r="D8" s="4">
+        <v>57</v>
+      </c>
+      <c r="E8" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>00039</v>
+      </c>
+      <c r="G8" s="4">
+        <v>107</v>
+      </c>
+      <c r="H8" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>0006B</v>
+      </c>
+      <c r="J8" s="4">
+        <v>157</v>
+      </c>
+      <c r="K8" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>0009D</v>
+      </c>
+      <c r="M8" s="4">
+        <v>207</v>
+      </c>
+      <c r="N8" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>000CF</v>
+      </c>
+      <c r="P8" s="4">
+        <v>257</v>
+      </c>
+      <c r="Q8" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>00101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>7</v>
+      </c>
+      <c r="B9" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>00007</v>
+      </c>
+      <c r="D9" s="4">
+        <v>58</v>
+      </c>
+      <c r="E9" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>0003A</v>
+      </c>
+      <c r="G9" s="4">
+        <v>108</v>
+      </c>
+      <c r="H9" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>0006C</v>
+      </c>
+      <c r="J9" s="4">
+        <v>158</v>
+      </c>
+      <c r="K9" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>0009E</v>
+      </c>
+      <c r="M9" s="4">
+        <v>208</v>
+      </c>
+      <c r="N9" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>000D0</v>
+      </c>
+      <c r="P9" s="4">
+        <v>258</v>
+      </c>
+      <c r="Q9" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>00102</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>8</v>
+      </c>
+      <c r="B10" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>00008</v>
+      </c>
+      <c r="D10" s="4">
+        <v>59</v>
+      </c>
+      <c r="E10" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>0003B</v>
+      </c>
+      <c r="G10" s="4">
+        <v>109</v>
+      </c>
+      <c r="H10" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>0006D</v>
+      </c>
+      <c r="J10" s="4">
+        <v>159</v>
+      </c>
+      <c r="K10" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>0009F</v>
+      </c>
+      <c r="M10" s="4">
+        <v>209</v>
+      </c>
+      <c r="N10" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>000D1</v>
+      </c>
+      <c r="P10" s="4">
+        <v>259</v>
+      </c>
+      <c r="Q10" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>00103</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>9</v>
+      </c>
+      <c r="B11" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>00009</v>
+      </c>
+      <c r="D11" s="4">
+        <v>60</v>
+      </c>
+      <c r="E11" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>0003C</v>
+      </c>
+      <c r="G11" s="4">
+        <v>110</v>
+      </c>
+      <c r="H11" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>0006E</v>
+      </c>
+      <c r="J11" s="4">
+        <v>160</v>
+      </c>
+      <c r="K11" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>000A0</v>
+      </c>
+      <c r="M11" s="4">
+        <v>210</v>
+      </c>
+      <c r="N11" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>000D2</v>
+      </c>
+      <c r="P11" s="4">
+        <v>260</v>
+      </c>
+      <c r="Q11" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>00104</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>10</v>
+      </c>
+      <c r="B12" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>0000A</v>
+      </c>
+      <c r="D12" s="4">
+        <v>61</v>
+      </c>
+      <c r="E12" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>0003D</v>
+      </c>
+      <c r="G12" s="4">
+        <v>111</v>
+      </c>
+      <c r="H12" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>0006F</v>
+      </c>
+      <c r="J12" s="4">
+        <v>161</v>
+      </c>
+      <c r="K12" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>000A1</v>
+      </c>
+      <c r="M12" s="4">
+        <v>211</v>
+      </c>
+      <c r="N12" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>000D3</v>
+      </c>
+      <c r="P12" s="4">
+        <v>261</v>
+      </c>
+      <c r="Q12" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>00105</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>11</v>
+      </c>
+      <c r="B13" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>0000B</v>
+      </c>
+      <c r="D13" s="4">
+        <v>62</v>
+      </c>
+      <c r="E13" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>0003E</v>
+      </c>
+      <c r="G13" s="4">
+        <v>112</v>
+      </c>
+      <c r="H13" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>00070</v>
+      </c>
+      <c r="J13" s="4">
+        <v>162</v>
+      </c>
+      <c r="K13" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>000A2</v>
+      </c>
+      <c r="M13" s="4">
+        <v>212</v>
+      </c>
+      <c r="N13" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>000D4</v>
+      </c>
+      <c r="P13" s="4">
+        <v>262</v>
+      </c>
+      <c r="Q13" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>00106</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>12</v>
+      </c>
+      <c r="B14" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>0000C</v>
+      </c>
+      <c r="D14" s="4">
+        <v>63</v>
+      </c>
+      <c r="E14" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>0003F</v>
+      </c>
+      <c r="G14" s="4">
+        <v>113</v>
+      </c>
+      <c r="H14" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>00071</v>
+      </c>
+      <c r="J14" s="4">
+        <v>163</v>
+      </c>
+      <c r="K14" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>000A3</v>
+      </c>
+      <c r="M14" s="4">
+        <v>213</v>
+      </c>
+      <c r="N14" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>000D5</v>
+      </c>
+      <c r="P14" s="4">
+        <v>263</v>
+      </c>
+      <c r="Q14" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>00107</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>13</v>
+      </c>
+      <c r="B15" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>0000D</v>
+      </c>
+      <c r="D15" s="4">
+        <v>64</v>
+      </c>
+      <c r="E15" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>00040</v>
+      </c>
+      <c r="G15" s="4">
+        <v>114</v>
+      </c>
+      <c r="H15" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>00072</v>
+      </c>
+      <c r="J15" s="4">
+        <v>164</v>
+      </c>
+      <c r="K15" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>000A4</v>
+      </c>
+      <c r="M15" s="4">
+        <v>214</v>
+      </c>
+      <c r="N15" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>000D6</v>
+      </c>
+      <c r="P15" s="4">
+        <v>264</v>
+      </c>
+      <c r="Q15" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>00108</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>14</v>
+      </c>
+      <c r="B16" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>0000E</v>
+      </c>
+      <c r="D16" s="4">
+        <v>65</v>
+      </c>
+      <c r="E16" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>00041</v>
+      </c>
+      <c r="G16" s="4">
+        <v>115</v>
+      </c>
+      <c r="H16" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>00073</v>
+      </c>
+      <c r="J16" s="4">
+        <v>165</v>
+      </c>
+      <c r="K16" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>000A5</v>
+      </c>
+      <c r="M16" s="4">
+        <v>215</v>
+      </c>
+      <c r="N16" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>000D7</v>
+      </c>
+      <c r="P16" s="4">
+        <v>265</v>
+      </c>
+      <c r="Q16" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>00109</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>15</v>
+      </c>
+      <c r="B17" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>0000F</v>
+      </c>
+      <c r="D17" s="4">
+        <v>66</v>
+      </c>
+      <c r="E17" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>00042</v>
+      </c>
+      <c r="G17" s="4">
+        <v>116</v>
+      </c>
+      <c r="H17" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>00074</v>
+      </c>
+      <c r="J17" s="4">
+        <v>166</v>
+      </c>
+      <c r="K17" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>000A6</v>
+      </c>
+      <c r="M17" s="4">
+        <v>216</v>
+      </c>
+      <c r="N17" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>000D8</v>
+      </c>
+      <c r="P17" s="4">
+        <v>266</v>
+      </c>
+      <c r="Q17" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>0010A</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>16</v>
+      </c>
+      <c r="B18" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>00010</v>
+      </c>
+      <c r="D18" s="4">
+        <v>67</v>
+      </c>
+      <c r="E18" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>00043</v>
+      </c>
+      <c r="G18" s="4">
+        <v>117</v>
+      </c>
+      <c r="H18" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>00075</v>
+      </c>
+      <c r="J18" s="4">
+        <v>167</v>
+      </c>
+      <c r="K18" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>000A7</v>
+      </c>
+      <c r="M18" s="4">
+        <v>217</v>
+      </c>
+      <c r="N18" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>000D9</v>
+      </c>
+      <c r="P18" s="4">
+        <v>267</v>
+      </c>
+      <c r="Q18" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>0010B</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>17</v>
+      </c>
+      <c r="B19" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>00011</v>
+      </c>
+      <c r="D19" s="4">
+        <v>68</v>
+      </c>
+      <c r="E19" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>00044</v>
+      </c>
+      <c r="G19" s="4">
+        <v>118</v>
+      </c>
+      <c r="H19" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>00076</v>
+      </c>
+      <c r="J19" s="4">
+        <v>168</v>
+      </c>
+      <c r="K19" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>000A8</v>
+      </c>
+      <c r="M19" s="4">
+        <v>218</v>
+      </c>
+      <c r="N19" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>000DA</v>
+      </c>
+      <c r="P19" s="4">
+        <v>268</v>
+      </c>
+      <c r="Q19" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>0010C</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>18</v>
+      </c>
+      <c r="B20" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>00012</v>
+      </c>
+      <c r="D20" s="4">
+        <v>69</v>
+      </c>
+      <c r="E20" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>00045</v>
+      </c>
+      <c r="G20" s="4">
+        <v>119</v>
+      </c>
+      <c r="H20" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>00077</v>
+      </c>
+      <c r="J20" s="4">
+        <v>169</v>
+      </c>
+      <c r="K20" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>000A9</v>
+      </c>
+      <c r="M20" s="4">
+        <v>219</v>
+      </c>
+      <c r="N20" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>000DB</v>
+      </c>
+      <c r="P20" s="4">
+        <v>269</v>
+      </c>
+      <c r="Q20" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>0010D</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>19</v>
+      </c>
+      <c r="B21" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>00013</v>
+      </c>
+      <c r="D21" s="4">
+        <v>70</v>
+      </c>
+      <c r="E21" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>00046</v>
+      </c>
+      <c r="G21" s="4">
+        <v>120</v>
+      </c>
+      <c r="H21" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>00078</v>
+      </c>
+      <c r="J21" s="4">
+        <v>170</v>
+      </c>
+      <c r="K21" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>000AA</v>
+      </c>
+      <c r="M21" s="4">
+        <v>220</v>
+      </c>
+      <c r="N21" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>000DC</v>
+      </c>
+      <c r="P21" s="4">
+        <v>270</v>
+      </c>
+      <c r="Q21" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>0010E</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>20</v>
+      </c>
+      <c r="B22" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>00014</v>
+      </c>
+      <c r="D22" s="4">
+        <v>71</v>
+      </c>
+      <c r="E22" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>00047</v>
+      </c>
+      <c r="G22" s="4">
+        <v>121</v>
+      </c>
+      <c r="H22" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>00079</v>
+      </c>
+      <c r="J22" s="4">
+        <v>171</v>
+      </c>
+      <c r="K22" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>000AB</v>
+      </c>
+      <c r="M22" s="4">
+        <v>221</v>
+      </c>
+      <c r="N22" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>000DD</v>
+      </c>
+      <c r="P22" s="4">
+        <v>271</v>
+      </c>
+      <c r="Q22" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>0010F</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
+        <v>21</v>
+      </c>
+      <c r="B23" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>00015</v>
+      </c>
+      <c r="D23" s="4">
+        <v>72</v>
+      </c>
+      <c r="E23" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>00048</v>
+      </c>
+      <c r="G23" s="4">
+        <v>122</v>
+      </c>
+      <c r="H23" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>0007A</v>
+      </c>
+      <c r="J23" s="4">
+        <v>172</v>
+      </c>
+      <c r="K23" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>000AC</v>
+      </c>
+      <c r="M23" s="4">
+        <v>222</v>
+      </c>
+      <c r="N23" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>000DE</v>
+      </c>
+      <c r="P23" s="4">
+        <v>272</v>
+      </c>
+      <c r="Q23" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>00110</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
+        <v>22</v>
+      </c>
+      <c r="B24" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>00016</v>
+      </c>
+      <c r="D24" s="4">
+        <v>73</v>
+      </c>
+      <c r="E24" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>00049</v>
+      </c>
+      <c r="G24" s="4">
+        <v>123</v>
+      </c>
+      <c r="H24" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>0007B</v>
+      </c>
+      <c r="J24" s="4">
+        <v>173</v>
+      </c>
+      <c r="K24" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>000AD</v>
+      </c>
+      <c r="M24" s="4">
+        <v>223</v>
+      </c>
+      <c r="N24" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>000DF</v>
+      </c>
+      <c r="P24" s="4">
+        <v>273</v>
+      </c>
+      <c r="Q24" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>00111</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
+        <v>23</v>
+      </c>
+      <c r="B25" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>00017</v>
+      </c>
+      <c r="D25" s="4">
+        <v>74</v>
+      </c>
+      <c r="E25" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>0004A</v>
+      </c>
+      <c r="G25" s="4">
+        <v>124</v>
+      </c>
+      <c r="H25" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>0007C</v>
+      </c>
+      <c r="J25" s="4">
+        <v>174</v>
+      </c>
+      <c r="K25" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>000AE</v>
+      </c>
+      <c r="M25" s="4">
+        <v>224</v>
+      </c>
+      <c r="N25" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>00000</v>
+      </c>
+      <c r="P25" s="4">
+        <v>274</v>
+      </c>
+      <c r="Q25" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>00112</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
+        <v>24</v>
+      </c>
+      <c r="B26" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>00018</v>
+      </c>
+      <c r="D26" s="4">
+        <v>75</v>
+      </c>
+      <c r="E26" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>0004B</v>
+      </c>
+      <c r="G26" s="4">
+        <v>125</v>
+      </c>
+      <c r="H26" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>0007D</v>
+      </c>
+      <c r="J26" s="4">
+        <v>175</v>
+      </c>
+      <c r="K26" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>000AF</v>
+      </c>
+      <c r="M26" s="4">
+        <v>225</v>
+      </c>
+      <c r="N26" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>00000</v>
+      </c>
+      <c r="P26" s="4">
+        <v>275</v>
+      </c>
+      <c r="Q26" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>00113</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
+        <v>25</v>
+      </c>
+      <c r="B27" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>00019</v>
+      </c>
+      <c r="D27" s="4">
+        <v>76</v>
+      </c>
+      <c r="E27" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>0004C</v>
+      </c>
+      <c r="G27" s="4">
+        <v>126</v>
+      </c>
+      <c r="H27" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>0007E</v>
+      </c>
+      <c r="J27" s="4">
+        <v>176</v>
+      </c>
+      <c r="K27" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>000B0</v>
+      </c>
+      <c r="M27" s="4">
+        <v>226</v>
+      </c>
+      <c r="N27" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>00000</v>
+      </c>
+      <c r="P27" s="4">
+        <v>276</v>
+      </c>
+      <c r="Q27" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>00114</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
+        <v>26</v>
+      </c>
+      <c r="B28" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>0001A</v>
+      </c>
+      <c r="D28" s="4">
+        <v>77</v>
+      </c>
+      <c r="E28" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>0004D</v>
+      </c>
+      <c r="G28" s="4">
+        <v>127</v>
+      </c>
+      <c r="H28" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>0007F</v>
+      </c>
+      <c r="J28" s="4">
+        <v>177</v>
+      </c>
+      <c r="K28" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>000B1</v>
+      </c>
+      <c r="M28" s="4">
+        <v>227</v>
+      </c>
+      <c r="N28" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>00000</v>
+      </c>
+      <c r="P28" s="4">
+        <v>277</v>
+      </c>
+      <c r="Q28" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>00115</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
+        <v>27</v>
+      </c>
+      <c r="B29" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>0001B</v>
+      </c>
+      <c r="D29" s="4">
+        <v>78</v>
+      </c>
+      <c r="E29" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>0004E</v>
+      </c>
+      <c r="G29" s="4">
+        <v>128</v>
+      </c>
+      <c r="H29" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>00080</v>
+      </c>
+      <c r="J29" s="4">
+        <v>178</v>
+      </c>
+      <c r="K29" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>000B2</v>
+      </c>
+      <c r="M29" s="4">
+        <v>228</v>
+      </c>
+      <c r="N29" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>00000</v>
+      </c>
+      <c r="P29" s="4">
+        <v>278</v>
+      </c>
+      <c r="Q29" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>00116</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A30" s="4">
+        <v>28</v>
+      </c>
+      <c r="B30" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>0001C</v>
+      </c>
+      <c r="D30" s="4">
+        <v>79</v>
+      </c>
+      <c r="E30" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>0004F</v>
+      </c>
+      <c r="G30" s="4">
+        <v>129</v>
+      </c>
+      <c r="H30" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>00081</v>
+      </c>
+      <c r="J30" s="4">
+        <v>179</v>
+      </c>
+      <c r="K30" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>000B3</v>
+      </c>
+      <c r="M30" s="4">
+        <v>229</v>
+      </c>
+      <c r="N30" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>00000</v>
+      </c>
+      <c r="P30" s="4">
+        <v>279</v>
+      </c>
+      <c r="Q30" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>00117</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
+        <v>29</v>
+      </c>
+      <c r="B31" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>0001D</v>
+      </c>
+      <c r="D31" s="4">
+        <v>80</v>
+      </c>
+      <c r="E31" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>00050</v>
+      </c>
+      <c r="G31" s="4">
+        <v>130</v>
+      </c>
+      <c r="H31" s="4" t="str">
+        <f>TEXT(DEC2HEX(G31, 5), "00000")</f>
+        <v>00082</v>
+      </c>
+      <c r="J31" s="4">
+        <v>180</v>
+      </c>
+      <c r="K31" s="4" t="str">
+        <f>TEXT(DEC2HEX(J31, 5), "00000")</f>
+        <v>000B4</v>
+      </c>
+      <c r="M31" s="4">
+        <v>230</v>
+      </c>
+      <c r="N31" s="4" t="str">
+        <f>TEXT(DEC2HEX(M31, 5), "00000")</f>
+        <v>00000</v>
+      </c>
+      <c r="P31" s="4">
+        <v>280</v>
+      </c>
+      <c r="Q31" s="4" t="str">
+        <f>TEXT(DEC2HEX(P31, 5), "00000")</f>
+        <v>00118</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A32" s="4">
+        <v>30</v>
+      </c>
+      <c r="B32" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>0001E</v>
+      </c>
+      <c r="D32" s="4">
+        <v>81</v>
+      </c>
+      <c r="E32" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>00051</v>
+      </c>
+      <c r="G32" s="4">
+        <v>131</v>
+      </c>
+      <c r="H32" s="4" t="str">
+        <f>TEXT(DEC2HEX(G32, 5), "00000")</f>
+        <v>00083</v>
+      </c>
+      <c r="J32" s="4">
+        <v>181</v>
+      </c>
+      <c r="K32" s="4" t="str">
+        <f>TEXT(DEC2HEX(J32, 5), "00000")</f>
+        <v>000B5</v>
+      </c>
+      <c r="M32" s="4">
+        <v>231</v>
+      </c>
+      <c r="N32" s="4" t="str">
+        <f>TEXT(DEC2HEX(M32, 5), "00000")</f>
+        <v>00000</v>
+      </c>
+      <c r="P32" s="4">
+        <v>281</v>
+      </c>
+      <c r="Q32" s="4" t="str">
+        <f>TEXT(DEC2HEX(P32, 5), "00000")</f>
+        <v>00119</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A33" s="4">
+        <v>31</v>
+      </c>
+      <c r="B33" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>0001F</v>
+      </c>
+      <c r="D33" s="4">
+        <v>82</v>
+      </c>
+      <c r="E33" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>00052</v>
+      </c>
+      <c r="G33" s="4">
+        <v>132</v>
+      </c>
+      <c r="H33" s="4" t="str">
+        <f t="shared" ref="H33:H51" si="6">TEXT(DEC2HEX(G33, 5), "00000")</f>
+        <v>00084</v>
+      </c>
+      <c r="J33" s="4">
+        <v>182</v>
+      </c>
+      <c r="K33" s="4" t="str">
+        <f t="shared" ref="K33:K51" si="7">TEXT(DEC2HEX(J33, 5), "00000")</f>
+        <v>000B6</v>
+      </c>
+      <c r="M33" s="4">
+        <v>232</v>
+      </c>
+      <c r="N33" s="4" t="str">
+        <f t="shared" ref="N33:N51" si="8">TEXT(DEC2HEX(M33, 5), "00000")</f>
+        <v>00000</v>
+      </c>
+      <c r="P33" s="4">
+        <v>282</v>
+      </c>
+      <c r="Q33" s="4" t="str">
+        <f t="shared" ref="Q33:Q51" si="9">TEXT(DEC2HEX(P33, 5), "00000")</f>
+        <v>0011A</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A34" s="4">
+        <v>32</v>
+      </c>
+      <c r="B34" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>00020</v>
+      </c>
+      <c r="D34" s="4">
+        <v>83</v>
+      </c>
+      <c r="E34" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>00053</v>
+      </c>
+      <c r="G34" s="4">
+        <v>133</v>
+      </c>
+      <c r="H34" s="4" t="str">
+        <f t="shared" si="6"/>
+        <v>00085</v>
+      </c>
+      <c r="J34" s="4">
+        <v>183</v>
+      </c>
+      <c r="K34" s="4" t="str">
+        <f t="shared" si="7"/>
+        <v>000B7</v>
+      </c>
+      <c r="M34" s="4">
+        <v>233</v>
+      </c>
+      <c r="N34" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>00000</v>
+      </c>
+      <c r="P34" s="4">
+        <v>283</v>
+      </c>
+      <c r="Q34" s="4" t="str">
+        <f t="shared" si="9"/>
+        <v>0011B</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A35" s="4">
+        <v>33</v>
+      </c>
+      <c r="B35" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>00021</v>
+      </c>
+      <c r="D35" s="4">
+        <v>84</v>
+      </c>
+      <c r="E35" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>00054</v>
+      </c>
+      <c r="G35" s="4">
+        <v>134</v>
+      </c>
+      <c r="H35" s="4" t="str">
+        <f t="shared" si="6"/>
+        <v>00086</v>
+      </c>
+      <c r="J35" s="4">
+        <v>184</v>
+      </c>
+      <c r="K35" s="4" t="str">
+        <f t="shared" si="7"/>
+        <v>000B8</v>
+      </c>
+      <c r="M35" s="4">
+        <v>234</v>
+      </c>
+      <c r="N35" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>000EA</v>
+      </c>
+      <c r="P35" s="4">
+        <v>284</v>
+      </c>
+      <c r="Q35" s="4" t="str">
+        <f t="shared" si="9"/>
+        <v>0011C</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A36" s="4">
+        <v>34</v>
+      </c>
+      <c r="B36" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>00022</v>
+      </c>
+      <c r="D36" s="4">
+        <v>85</v>
+      </c>
+      <c r="E36" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>00055</v>
+      </c>
+      <c r="G36" s="4">
+        <v>135</v>
+      </c>
+      <c r="H36" s="4" t="str">
+        <f t="shared" si="6"/>
+        <v>00087</v>
+      </c>
+      <c r="J36" s="4">
+        <v>185</v>
+      </c>
+      <c r="K36" s="4" t="str">
+        <f t="shared" si="7"/>
+        <v>000B9</v>
+      </c>
+      <c r="M36" s="4">
+        <v>235</v>
+      </c>
+      <c r="N36" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>000EB</v>
+      </c>
+      <c r="P36" s="4">
+        <v>285</v>
+      </c>
+      <c r="Q36" s="4" t="str">
+        <f t="shared" si="9"/>
+        <v>0011D</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A37" s="4">
+        <v>35</v>
+      </c>
+      <c r="B37" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>00023</v>
+      </c>
+      <c r="D37" s="4">
+        <v>86</v>
+      </c>
+      <c r="E37" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>00056</v>
+      </c>
+      <c r="G37" s="4">
+        <v>136</v>
+      </c>
+      <c r="H37" s="4" t="str">
+        <f t="shared" si="6"/>
+        <v>00088</v>
+      </c>
+      <c r="J37" s="4">
+        <v>186</v>
+      </c>
+      <c r="K37" s="4" t="str">
+        <f t="shared" si="7"/>
+        <v>000BA</v>
+      </c>
+      <c r="M37" s="4">
+        <v>236</v>
+      </c>
+      <c r="N37" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>000EC</v>
+      </c>
+      <c r="P37" s="4">
+        <v>286</v>
+      </c>
+      <c r="Q37" s="4" t="str">
+        <f t="shared" si="9"/>
+        <v>0011E</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A38" s="4">
+        <v>36</v>
+      </c>
+      <c r="B38" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>00024</v>
+      </c>
+      <c r="D38" s="4">
+        <v>87</v>
+      </c>
+      <c r="E38" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>00057</v>
+      </c>
+      <c r="G38" s="4">
+        <v>137</v>
+      </c>
+      <c r="H38" s="4" t="str">
+        <f t="shared" si="6"/>
+        <v>00089</v>
+      </c>
+      <c r="J38" s="4">
+        <v>187</v>
+      </c>
+      <c r="K38" s="4" t="str">
+        <f t="shared" si="7"/>
+        <v>000BB</v>
+      </c>
+      <c r="M38" s="4">
+        <v>237</v>
+      </c>
+      <c r="N38" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>000ED</v>
+      </c>
+      <c r="P38" s="4">
+        <v>287</v>
+      </c>
+      <c r="Q38" s="4" t="str">
+        <f t="shared" si="9"/>
+        <v>0011F</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A39" s="4">
+        <v>37</v>
+      </c>
+      <c r="B39" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>00025</v>
+      </c>
+      <c r="D39" s="4">
+        <v>88</v>
+      </c>
+      <c r="E39" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>00058</v>
+      </c>
+      <c r="G39" s="4">
+        <v>138</v>
+      </c>
+      <c r="H39" s="4" t="str">
+        <f t="shared" si="6"/>
+        <v>0008A</v>
+      </c>
+      <c r="J39" s="4">
+        <v>188</v>
+      </c>
+      <c r="K39" s="4" t="str">
+        <f t="shared" si="7"/>
+        <v>000BC</v>
+      </c>
+      <c r="M39" s="4">
+        <v>238</v>
+      </c>
+      <c r="N39" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>000EE</v>
+      </c>
+      <c r="P39" s="4">
+        <v>288</v>
+      </c>
+      <c r="Q39" s="4" t="str">
+        <f t="shared" si="9"/>
+        <v>00120</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A40" s="4">
+        <v>38</v>
+      </c>
+      <c r="B40" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>00026</v>
+      </c>
+      <c r="D40" s="4">
+        <v>89</v>
+      </c>
+      <c r="E40" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>00059</v>
+      </c>
+      <c r="G40" s="4">
+        <v>139</v>
+      </c>
+      <c r="H40" s="4" t="str">
+        <f t="shared" si="6"/>
+        <v>0008B</v>
+      </c>
+      <c r="J40" s="4">
+        <v>189</v>
+      </c>
+      <c r="K40" s="4" t="str">
+        <f t="shared" si="7"/>
+        <v>000BD</v>
+      </c>
+      <c r="M40" s="4">
+        <v>239</v>
+      </c>
+      <c r="N40" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>000EF</v>
+      </c>
+      <c r="P40" s="4">
+        <v>289</v>
+      </c>
+      <c r="Q40" s="4" t="str">
+        <f t="shared" si="9"/>
+        <v>00121</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A41" s="4">
+        <v>39</v>
+      </c>
+      <c r="B41" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>00027</v>
+      </c>
+      <c r="D41" s="4">
+        <v>90</v>
+      </c>
+      <c r="E41" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>0005A</v>
+      </c>
+      <c r="G41" s="4">
+        <v>140</v>
+      </c>
+      <c r="H41" s="4" t="str">
+        <f t="shared" si="6"/>
+        <v>0008C</v>
+      </c>
+      <c r="J41" s="4">
+        <v>190</v>
+      </c>
+      <c r="K41" s="4" t="str">
+        <f t="shared" si="7"/>
+        <v>000BE</v>
+      </c>
+      <c r="M41" s="4">
+        <v>240</v>
+      </c>
+      <c r="N41" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>000F0</v>
+      </c>
+      <c r="P41" s="4">
+        <v>290</v>
+      </c>
+      <c r="Q41" s="4" t="str">
+        <f t="shared" si="9"/>
+        <v>00122</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A42" s="4">
+        <v>40</v>
+      </c>
+      <c r="B42" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>00028</v>
+      </c>
+      <c r="D42" s="4">
+        <v>91</v>
+      </c>
+      <c r="E42" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>0005B</v>
+      </c>
+      <c r="G42" s="4">
+        <v>141</v>
+      </c>
+      <c r="H42" s="4" t="str">
+        <f t="shared" si="6"/>
+        <v>0008D</v>
+      </c>
+      <c r="J42" s="4">
+        <v>191</v>
+      </c>
+      <c r="K42" s="4" t="str">
+        <f t="shared" si="7"/>
+        <v>000BF</v>
+      </c>
+      <c r="M42" s="4">
+        <v>241</v>
+      </c>
+      <c r="N42" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>000F1</v>
+      </c>
+      <c r="P42" s="4">
+        <v>291</v>
+      </c>
+      <c r="Q42" s="4" t="str">
+        <f t="shared" si="9"/>
+        <v>00123</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A43" s="4">
+        <v>41</v>
+      </c>
+      <c r="B43" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>00029</v>
+      </c>
+      <c r="D43" s="4">
+        <v>92</v>
+      </c>
+      <c r="E43" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>0005C</v>
+      </c>
+      <c r="G43" s="4">
+        <v>142</v>
+      </c>
+      <c r="H43" s="4" t="str">
+        <f t="shared" si="6"/>
+        <v>0008E</v>
+      </c>
+      <c r="J43" s="4">
+        <v>192</v>
+      </c>
+      <c r="K43" s="4" t="str">
+        <f t="shared" si="7"/>
+        <v>000C0</v>
+      </c>
+      <c r="M43" s="4">
+        <v>242</v>
+      </c>
+      <c r="N43" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>000F2</v>
+      </c>
+      <c r="P43" s="4">
+        <v>292</v>
+      </c>
+      <c r="Q43" s="4" t="str">
+        <f t="shared" si="9"/>
+        <v>00124</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A44" s="4">
+        <v>42</v>
+      </c>
+      <c r="B44" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>0002A</v>
+      </c>
+      <c r="D44" s="4">
+        <v>93</v>
+      </c>
+      <c r="E44" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>0005D</v>
+      </c>
+      <c r="G44" s="4">
+        <v>143</v>
+      </c>
+      <c r="H44" s="4" t="str">
+        <f t="shared" si="6"/>
+        <v>0008F</v>
+      </c>
+      <c r="J44" s="4">
+        <v>193</v>
+      </c>
+      <c r="K44" s="4" t="str">
+        <f t="shared" si="7"/>
+        <v>000C1</v>
+      </c>
+      <c r="M44" s="4">
+        <v>243</v>
+      </c>
+      <c r="N44" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>000F3</v>
+      </c>
+      <c r="P44" s="4">
+        <v>293</v>
+      </c>
+      <c r="Q44" s="4" t="str">
+        <f t="shared" si="9"/>
+        <v>00125</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A45" s="4">
+        <v>43</v>
+      </c>
+      <c r="B45" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>0002B</v>
+      </c>
+      <c r="D45" s="4">
+        <v>94</v>
+      </c>
+      <c r="E45" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>0005E</v>
+      </c>
+      <c r="G45" s="4">
+        <v>144</v>
+      </c>
+      <c r="H45" s="4" t="str">
+        <f t="shared" si="6"/>
+        <v>00090</v>
+      </c>
+      <c r="J45" s="4">
+        <v>194</v>
+      </c>
+      <c r="K45" s="4" t="str">
+        <f t="shared" si="7"/>
+        <v>000C2</v>
+      </c>
+      <c r="M45" s="4">
+        <v>244</v>
+      </c>
+      <c r="N45" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>000F4</v>
+      </c>
+      <c r="P45" s="4">
+        <v>294</v>
+      </c>
+      <c r="Q45" s="4" t="str">
+        <f t="shared" si="9"/>
+        <v>00126</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A46" s="4">
+        <v>44</v>
+      </c>
+      <c r="B46" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>0002C</v>
+      </c>
+      <c r="D46" s="4">
+        <v>95</v>
+      </c>
+      <c r="E46" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>0005F</v>
+      </c>
+      <c r="G46" s="4">
+        <v>145</v>
+      </c>
+      <c r="H46" s="4" t="str">
+        <f t="shared" si="6"/>
+        <v>00091</v>
+      </c>
+      <c r="J46" s="4">
+        <v>195</v>
+      </c>
+      <c r="K46" s="4" t="str">
+        <f t="shared" si="7"/>
+        <v>000C3</v>
+      </c>
+      <c r="M46" s="4">
+        <v>245</v>
+      </c>
+      <c r="N46" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>000F5</v>
+      </c>
+      <c r="P46" s="4">
+        <v>295</v>
+      </c>
+      <c r="Q46" s="4" t="str">
+        <f t="shared" si="9"/>
+        <v>00127</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A47" s="4">
+        <v>45</v>
+      </c>
+      <c r="B47" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>0002D</v>
+      </c>
+      <c r="D47" s="4">
+        <v>96</v>
+      </c>
+      <c r="E47" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>00060</v>
+      </c>
+      <c r="G47" s="4">
+        <v>146</v>
+      </c>
+      <c r="H47" s="4" t="str">
+        <f t="shared" si="6"/>
+        <v>00092</v>
+      </c>
+      <c r="J47" s="4">
+        <v>196</v>
+      </c>
+      <c r="K47" s="4" t="str">
+        <f t="shared" si="7"/>
+        <v>000C4</v>
+      </c>
+      <c r="M47" s="4">
+        <v>246</v>
+      </c>
+      <c r="N47" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>000F6</v>
+      </c>
+      <c r="P47" s="4">
+        <v>296</v>
+      </c>
+      <c r="Q47" s="4" t="str">
+        <f t="shared" si="9"/>
+        <v>00128</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A48" s="4">
+        <v>46</v>
+      </c>
+      <c r="B48" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>0002E</v>
+      </c>
+      <c r="D48" s="4">
+        <v>97</v>
+      </c>
+      <c r="E48" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>00061</v>
+      </c>
+      <c r="G48" s="4">
+        <v>147</v>
+      </c>
+      <c r="H48" s="4" t="str">
+        <f t="shared" si="6"/>
+        <v>00093</v>
+      </c>
+      <c r="J48" s="4">
+        <v>197</v>
+      </c>
+      <c r="K48" s="4" t="str">
+        <f t="shared" si="7"/>
+        <v>000C5</v>
+      </c>
+      <c r="M48" s="4">
+        <v>247</v>
+      </c>
+      <c r="N48" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>000F7</v>
+      </c>
+      <c r="P48" s="4">
+        <v>297</v>
+      </c>
+      <c r="Q48" s="4" t="str">
+        <f t="shared" si="9"/>
+        <v>00129</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A49" s="4">
+        <v>47</v>
+      </c>
+      <c r="B49" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>0002F</v>
+      </c>
+      <c r="D49" s="4">
+        <v>98</v>
+      </c>
+      <c r="E49" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>00062</v>
+      </c>
+      <c r="G49" s="4">
+        <v>148</v>
+      </c>
+      <c r="H49" s="4" t="str">
+        <f t="shared" si="6"/>
+        <v>00094</v>
+      </c>
+      <c r="J49" s="4">
+        <v>198</v>
+      </c>
+      <c r="K49" s="4" t="str">
+        <f t="shared" si="7"/>
+        <v>000C6</v>
+      </c>
+      <c r="M49" s="4">
+        <v>248</v>
+      </c>
+      <c r="N49" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>000F8</v>
+      </c>
+      <c r="P49" s="4">
+        <v>298</v>
+      </c>
+      <c r="Q49" s="4" t="str">
+        <f t="shared" si="9"/>
+        <v>0012A</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A50" s="4">
+        <v>48</v>
+      </c>
+      <c r="B50" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>00030</v>
+      </c>
+      <c r="D50" s="4">
+        <v>99</v>
+      </c>
+      <c r="E50" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>00063</v>
+      </c>
+      <c r="G50" s="4">
+        <v>149</v>
+      </c>
+      <c r="H50" s="4" t="str">
+        <f t="shared" si="6"/>
+        <v>00095</v>
+      </c>
+      <c r="J50" s="4">
+        <v>199</v>
+      </c>
+      <c r="K50" s="4" t="str">
+        <f t="shared" si="7"/>
+        <v>000C7</v>
+      </c>
+      <c r="M50" s="4">
+        <v>249</v>
+      </c>
+      <c r="N50" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>000F9</v>
+      </c>
+      <c r="P50" s="4">
+        <v>299</v>
+      </c>
+      <c r="Q50" s="4" t="str">
+        <f t="shared" si="9"/>
+        <v>0012B</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A51" s="4">
+        <v>49</v>
+      </c>
+      <c r="B51" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>00031</v>
+      </c>
+      <c r="D51" s="4">
+        <v>100</v>
+      </c>
+      <c r="E51" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>00064</v>
+      </c>
+      <c r="G51" s="4">
+        <v>150</v>
+      </c>
+      <c r="H51" s="4" t="str">
+        <f t="shared" si="6"/>
+        <v>00096</v>
+      </c>
+      <c r="J51" s="4">
+        <v>200</v>
+      </c>
+      <c r="K51" s="4" t="str">
+        <f t="shared" si="7"/>
+        <v>000C8</v>
+      </c>
+      <c r="M51" s="4">
+        <v>250</v>
+      </c>
+      <c r="N51" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>000FA</v>
+      </c>
+      <c r="P51" s="4">
+        <v>300</v>
+      </c>
+      <c r="Q51" s="4" t="str">
+        <f t="shared" si="9"/>
+        <v>0012C</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A52" s="4">
+        <v>50</v>
+      </c>
+      <c r="B52" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>00032</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="B1:D1 B3 B4:C26 E17:E23 B27:D1048576">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+  <conditionalFormatting sqref="A60:C1048576 C27:C59 A3:A59 A1:E1">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
       <formula>"N"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+      <formula>"D"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G1:H1">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+      <formula>"D"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J1:K1">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+      <formula>"D"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M1:N1">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+      <formula>"D"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P1:Q1">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"D"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1278,10 +3639,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A17:E23">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
       <formula>"N"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
       <formula>"D"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1291,21 +3652,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A855378936633F46935DE081F3F0A723" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6fb8377a16f57469f31fda63402737be">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="0e1bb11d-1fe8-4e80-a80d-c671e8cd2a50" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a5a807ddb17e97ebd5eac858e2e697fd" ns3:_="">
     <xsd:import namespace="0e1bb11d-1fe8-4e80-a80d-c671e8cd2a50"/>
@@ -1507,10 +3853,35 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DF4A1F3-27F5-4026-9F7B-EA2EEA754838}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8A8016DE-DC46-404F-9AC8-AB31FBBA1BB2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="0e1bb11d-1fe8-4e80-a80d-c671e8cd2a50"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1532,19 +3903,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8A8016DE-DC46-404F-9AC8-AB31FBBA1BB2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DF4A1F3-27F5-4026-9F7B-EA2EEA754838}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="0e1bb11d-1fe8-4e80-a80d-c671e8cd2a50"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Working: Updated Sql Structure
</commit_message>
<xml_diff>
--- a/FullStackProject/documentation/serverAPIs.xlsx
+++ b/FullStackProject/documentation/serverAPIs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Html_CSS\FullStackProject\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3AB4690-33D2-4026-A730-63E15E2A7D42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1FDD785-AC77-49C5-AD05-14F21DA38276}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="16305" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4605" yWindow="3315" windowWidth="21600" windowHeight="11835" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Error Code" sheetId="17" r:id="rId1"/>
@@ -1335,7 +1335,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1388,7 +1388,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2230,8 +2233,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8787874B-90D5-45F1-9880-0373B280E830}">
   <dimension ref="A1:R52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2783,7 +2786,7 @@
       <c r="A13" s="15">
         <v>11</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="16" t="s">
         <v>153</v>
       </c>
       <c r="C13" s="14"/>
@@ -2827,7 +2830,7 @@
       <c r="A14" s="15">
         <v>12</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="16" t="s">
         <v>159</v>
       </c>
       <c r="C14" s="14"/>
@@ -4570,8 +4573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCCF9E71-D3B5-42A3-9DB3-24557FECF4AE}">
   <dimension ref="A1:G500"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4759,10 +4762,10 @@
       <c r="D9" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="19" t="s">
         <v>382</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="19" t="s">
         <v>380</v>
       </c>
       <c r="G9" s="1" t="s">
@@ -8963,6 +8966,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A855378936633F46935DE081F3F0A723" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6fb8377a16f57469f31fda63402737be">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="0e1bb11d-1fe8-4e80-a80d-c671e8cd2a50" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a5a807ddb17e97ebd5eac858e2e697fd" ns3:_="">
     <xsd:import namespace="0e1bb11d-1fe8-4e80-a80d-c671e8cd2a50"/>
@@ -9164,22 +9182,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{88BC72A4-2999-4A2E-B325-3F14F9A9DFDC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="0e1bb11d-1fe8-4e80-a80d-c671e8cd2a50"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DF4A1F3-27F5-4026-9F7B-EA2EEA754838}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8A8016DE-DC46-404F-9AC8-AB31FBBA1BB2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9195,28 +9222,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DF4A1F3-27F5-4026-9F7B-EA2EEA754838}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{88BC72A4-2999-4A2E-B325-3F14F9A9DFDC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="0e1bb11d-1fe8-4e80-a80d-c671e8cd2a50"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Created : Add Chat & groupChat APIs
</commit_message>
<xml_diff>
--- a/FullStackProject/documentation/serverAPIs.xlsx
+++ b/FullStackProject/documentation/serverAPIs.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Html_CSS\FullStackProject\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD8C3738-2A0C-45CD-830E-F05C9E4F688C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67345C84-F110-4B00-8D12-91EFD0C213AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4605" yWindow="3315" windowWidth="21600" windowHeight="11835" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Error Code" sheetId="17" r:id="rId1"/>
     <sheet name="Status Code" sheetId="15" r:id="rId2"/>
-    <sheet name="Chat APIs" sheetId="18" r:id="rId3"/>
+    <sheet name="APIs" sheetId="19" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="400">
   <si>
     <t xml:space="preserve">Sr </t>
   </si>
@@ -46,9 +46,6 @@
     <t>Code</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
     <t>Error</t>
   </si>
   <si>
@@ -1235,6 +1232,12 @@
   </si>
   <si>
     <t>Add payment to the chat &amp; payment table</t>
+  </si>
+  <si>
+    <t>Folder Name</t>
+  </si>
+  <si>
+    <t>Response Codes</t>
   </si>
 </sst>
 </file>
@@ -1288,7 +1291,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1304,6 +1307,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1335,7 +1344,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1390,6 +1399,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1836,10 +1848,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="8" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1847,7 +1859,7 @@
     </row>
     <row r="3" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1855,10 +1867,10 @@
         <v>200</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1866,10 +1878,10 @@
         <v>201</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1877,10 +1889,10 @@
         <v>202</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1888,10 +1900,10 @@
         <v>203</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="10" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1900,7 +1912,7 @@
     </row>
     <row r="9" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1908,10 +1920,10 @@
         <v>400</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1919,10 +1931,10 @@
         <v>401</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1930,10 +1942,10 @@
         <v>403</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1941,10 +1953,10 @@
         <v>404</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1952,10 +1964,10 @@
         <v>405</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1963,10 +1975,10 @@
         <v>406</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1974,10 +1986,10 @@
         <v>408</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1985,10 +1997,10 @@
         <v>409</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1996,10 +2008,10 @@
         <v>410</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2007,10 +2019,10 @@
         <v>411</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2018,10 +2030,10 @@
         <v>413</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2029,10 +2041,10 @@
         <v>414</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2040,10 +2052,10 @@
         <v>415</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="2:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2051,10 +2063,10 @@
         <v>422</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="2:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2062,10 +2074,10 @@
         <v>429</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="2:4" s="10" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2073,7 +2085,7 @@
     </row>
     <row r="26" spans="2:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C26" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="27" spans="2:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2081,10 +2093,10 @@
         <v>500</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="2:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2092,10 +2104,10 @@
         <v>501</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29" spans="2:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2103,10 +2115,10 @@
         <v>502</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="30" spans="2:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2114,10 +2126,10 @@
         <v>503</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="31" spans="2:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2125,10 +2137,10 @@
         <v>504</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="32" spans="2:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2136,10 +2148,10 @@
         <v>505</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="33" spans="2:4" s="10" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2147,7 +2159,7 @@
     </row>
     <row r="34" spans="2:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C34" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="35" spans="2:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2155,10 +2167,10 @@
         <v>301</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="36" spans="2:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2166,10 +2178,10 @@
         <v>302</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="37" spans="2:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2177,10 +2189,10 @@
         <v>303</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="38" spans="2:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2188,10 +2200,10 @@
         <v>304</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="39" spans="2:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2199,10 +2211,10 @@
         <v>307</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="40" spans="2:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2210,10 +2222,10 @@
         <v>308</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -2234,7 +2246,7 @@
   <dimension ref="A1:R52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2256,42 +2268,42 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="14"/>
       <c r="D1" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E1" s="13" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="14"/>
       <c r="G1" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H1" s="13" t="s">
         <v>1</v>
       </c>
       <c r="I1" s="14"/>
       <c r="J1" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K1" s="13" t="s">
         <v>1</v>
       </c>
       <c r="L1" s="14"/>
       <c r="M1" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="N1" s="13" t="s">
         <v>1</v>
       </c>
       <c r="O1" s="14"/>
       <c r="P1" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="Q1" s="13" t="s">
         <v>1</v>
@@ -2303,42 +2315,42 @@
         <v>0</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C2" s="14"/>
       <c r="D2" s="15">
         <v>51</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F2" s="14"/>
       <c r="G2" s="15">
         <v>101</v>
       </c>
       <c r="H2" s="15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I2" s="14"/>
       <c r="J2" s="15">
         <v>151</v>
       </c>
       <c r="K2" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L2" s="14"/>
       <c r="M2" s="15">
         <v>201</v>
       </c>
       <c r="N2" s="15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="O2" s="14"/>
       <c r="P2" s="15">
         <v>251</v>
       </c>
       <c r="Q2" s="15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="R2" s="14"/>
     </row>
@@ -2347,42 +2359,42 @@
         <v>1</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C3" s="14"/>
       <c r="D3" s="15">
         <v>52</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F3" s="14"/>
       <c r="G3" s="15">
         <v>102</v>
       </c>
       <c r="H3" s="15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I3" s="14"/>
       <c r="J3" s="15">
         <v>152</v>
       </c>
       <c r="K3" s="15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L3" s="14"/>
       <c r="M3" s="15">
         <v>202</v>
       </c>
       <c r="N3" s="15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="O3" s="14"/>
       <c r="P3" s="15">
         <v>252</v>
       </c>
       <c r="Q3" s="15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="R3" s="14"/>
     </row>
@@ -2391,42 +2403,42 @@
         <v>2</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C4" s="14"/>
       <c r="D4" s="15">
         <v>53</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F4" s="14"/>
       <c r="G4" s="15">
         <v>103</v>
       </c>
       <c r="H4" s="15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I4" s="14"/>
       <c r="J4" s="15">
         <v>153</v>
       </c>
       <c r="K4" s="15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L4" s="14"/>
       <c r="M4" s="15">
         <v>203</v>
       </c>
       <c r="N4" s="15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O4" s="14"/>
       <c r="P4" s="15">
         <v>253</v>
       </c>
       <c r="Q4" s="15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="R4" s="14"/>
     </row>
@@ -2435,42 +2447,42 @@
         <v>3</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="15">
         <v>54</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F5" s="14"/>
       <c r="G5" s="15">
         <v>104</v>
       </c>
       <c r="H5" s="15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I5" s="14"/>
       <c r="J5" s="15">
         <v>154</v>
       </c>
       <c r="K5" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="L5" s="14"/>
       <c r="M5" s="15">
         <v>204</v>
       </c>
       <c r="N5" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="O5" s="14"/>
       <c r="P5" s="15">
         <v>254</v>
       </c>
       <c r="Q5" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="R5" s="14"/>
     </row>
@@ -2479,42 +2491,42 @@
         <v>4</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="15">
         <v>55</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F6" s="14"/>
       <c r="G6" s="15">
         <v>105</v>
       </c>
       <c r="H6" s="15" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I6" s="14"/>
       <c r="J6" s="15">
         <v>155</v>
       </c>
       <c r="K6" s="15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L6" s="14"/>
       <c r="M6" s="15">
         <v>205</v>
       </c>
       <c r="N6" s="15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="O6" s="14"/>
       <c r="P6" s="15">
         <v>255</v>
       </c>
       <c r="Q6" s="15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="R6" s="14"/>
     </row>
@@ -2523,42 +2535,42 @@
         <v>5</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="15">
         <v>56</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F7" s="14"/>
       <c r="G7" s="15">
         <v>106</v>
       </c>
       <c r="H7" s="15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I7" s="14"/>
       <c r="J7" s="15">
         <v>156</v>
       </c>
       <c r="K7" s="15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="L7" s="14"/>
       <c r="M7" s="15">
         <v>206</v>
       </c>
       <c r="N7" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="O7" s="14"/>
       <c r="P7" s="15">
         <v>256</v>
       </c>
       <c r="Q7" s="15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="R7" s="14"/>
     </row>
@@ -2567,42 +2579,42 @@
         <v>6</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C8" s="14"/>
       <c r="D8" s="15">
         <v>57</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F8" s="14"/>
       <c r="G8" s="15">
         <v>107</v>
       </c>
       <c r="H8" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I8" s="14"/>
       <c r="J8" s="15">
         <v>157</v>
       </c>
       <c r="K8" s="15" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L8" s="14"/>
       <c r="M8" s="15">
         <v>207</v>
       </c>
       <c r="N8" s="15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="O8" s="14"/>
       <c r="P8" s="15">
         <v>257</v>
       </c>
       <c r="Q8" s="15" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="R8" s="14"/>
     </row>
@@ -2611,42 +2623,42 @@
         <v>7</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C9" s="14"/>
       <c r="D9" s="15">
         <v>58</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F9" s="14"/>
       <c r="G9" s="15">
         <v>108</v>
       </c>
       <c r="H9" s="15" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I9" s="14"/>
       <c r="J9" s="15">
         <v>158</v>
       </c>
       <c r="K9" s="15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L9" s="14"/>
       <c r="M9" s="15">
         <v>208</v>
       </c>
       <c r="N9" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="O9" s="14"/>
       <c r="P9" s="15">
         <v>258</v>
       </c>
       <c r="Q9" s="15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="R9" s="14"/>
     </row>
@@ -2655,42 +2667,42 @@
         <v>8</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C10" s="14"/>
       <c r="D10" s="15">
         <v>59</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F10" s="14"/>
       <c r="G10" s="15">
         <v>109</v>
       </c>
       <c r="H10" s="15" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="I10" s="14"/>
       <c r="J10" s="15">
         <v>159</v>
       </c>
       <c r="K10" s="15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L10" s="14"/>
       <c r="M10" s="15">
         <v>209</v>
       </c>
       <c r="N10" s="15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="O10" s="14"/>
       <c r="P10" s="15">
         <v>259</v>
       </c>
       <c r="Q10" s="15" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="R10" s="14"/>
     </row>
@@ -2699,42 +2711,42 @@
         <v>9</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C11" s="14"/>
       <c r="D11" s="15">
         <v>60</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F11" s="14"/>
       <c r="G11" s="15">
         <v>110</v>
       </c>
       <c r="H11" s="15" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I11" s="14"/>
       <c r="J11" s="15">
         <v>160</v>
       </c>
       <c r="K11" s="15" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="L11" s="14"/>
       <c r="M11" s="15">
         <v>210</v>
       </c>
       <c r="N11" s="15" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="O11" s="14"/>
       <c r="P11" s="15">
         <v>260</v>
       </c>
       <c r="Q11" s="15" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="R11" s="14"/>
     </row>
@@ -2743,42 +2755,42 @@
         <v>10</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C12" s="14"/>
       <c r="D12" s="15">
         <v>61</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F12" s="14"/>
       <c r="G12" s="15">
         <v>111</v>
       </c>
       <c r="H12" s="15" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I12" s="14"/>
       <c r="J12" s="15">
         <v>161</v>
       </c>
       <c r="K12" s="15" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L12" s="14"/>
       <c r="M12" s="15">
         <v>211</v>
       </c>
       <c r="N12" s="15" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="O12" s="14"/>
       <c r="P12" s="15">
         <v>261</v>
       </c>
       <c r="Q12" s="15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="R12" s="14"/>
     </row>
@@ -2787,42 +2799,42 @@
         <v>11</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C13" s="14"/>
       <c r="D13" s="15">
         <v>62</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F13" s="14"/>
       <c r="G13" s="15">
         <v>112</v>
       </c>
       <c r="H13" s="15" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I13" s="14"/>
       <c r="J13" s="15">
         <v>162</v>
       </c>
       <c r="K13" s="15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L13" s="14"/>
       <c r="M13" s="15">
         <v>212</v>
       </c>
       <c r="N13" s="15" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="O13" s="14"/>
       <c r="P13" s="15">
         <v>262</v>
       </c>
       <c r="Q13" s="15" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="R13" s="14"/>
     </row>
@@ -2831,42 +2843,42 @@
         <v>12</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C14" s="14"/>
       <c r="D14" s="15">
         <v>63</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F14" s="14"/>
       <c r="G14" s="15">
         <v>113</v>
       </c>
       <c r="H14" s="15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I14" s="14"/>
       <c r="J14" s="15">
         <v>163</v>
       </c>
       <c r="K14" s="15" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L14" s="14"/>
       <c r="M14" s="15">
         <v>213</v>
       </c>
       <c r="N14" s="15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="O14" s="14"/>
       <c r="P14" s="15">
         <v>263</v>
       </c>
       <c r="Q14" s="15" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="R14" s="14"/>
     </row>
@@ -2875,42 +2887,42 @@
         <v>13</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C15" s="14"/>
       <c r="D15" s="15">
         <v>64</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F15" s="14"/>
       <c r="G15" s="15">
         <v>114</v>
       </c>
       <c r="H15" s="15" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I15" s="14"/>
       <c r="J15" s="15">
         <v>164</v>
       </c>
       <c r="K15" s="15" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L15" s="14"/>
       <c r="M15" s="15">
         <v>214</v>
       </c>
       <c r="N15" s="15" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="O15" s="14"/>
       <c r="P15" s="15">
         <v>264</v>
       </c>
       <c r="Q15" s="15" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="R15" s="14"/>
     </row>
@@ -2919,42 +2931,42 @@
         <v>14</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C16" s="14"/>
       <c r="D16" s="15">
         <v>65</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F16" s="14"/>
       <c r="G16" s="15">
         <v>115</v>
       </c>
       <c r="H16" s="15" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="I16" s="14"/>
       <c r="J16" s="15">
         <v>165</v>
       </c>
       <c r="K16" s="15" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="L16" s="14"/>
       <c r="M16" s="15">
         <v>215</v>
       </c>
       <c r="N16" s="15" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="O16" s="14"/>
       <c r="P16" s="15">
         <v>265</v>
       </c>
       <c r="Q16" s="15" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="R16" s="14"/>
     </row>
@@ -2962,43 +2974,43 @@
       <c r="A17" s="15">
         <v>15</v>
       </c>
-      <c r="B17" s="15" t="s">
-        <v>177</v>
+      <c r="B17" s="16" t="s">
+        <v>176</v>
       </c>
       <c r="C17" s="14"/>
       <c r="D17" s="15">
         <v>66</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F17" s="14"/>
       <c r="G17" s="15">
         <v>116</v>
       </c>
       <c r="H17" s="15" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I17" s="14"/>
       <c r="J17" s="15">
         <v>166</v>
       </c>
       <c r="K17" s="15" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="L17" s="14"/>
       <c r="M17" s="15">
         <v>216</v>
       </c>
       <c r="N17" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="O17" s="14"/>
       <c r="P17" s="15">
         <v>266</v>
       </c>
       <c r="Q17" s="15" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="R17" s="14"/>
     </row>
@@ -3006,43 +3018,43 @@
       <c r="A18" s="15">
         <v>16</v>
       </c>
-      <c r="B18" s="15" t="s">
-        <v>183</v>
+      <c r="B18" s="16" t="s">
+        <v>182</v>
       </c>
       <c r="C18" s="14"/>
       <c r="D18" s="15">
         <v>67</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F18" s="14"/>
       <c r="G18" s="15">
         <v>117</v>
       </c>
       <c r="H18" s="15" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="I18" s="14"/>
       <c r="J18" s="15">
         <v>167</v>
       </c>
       <c r="K18" s="15" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="L18" s="14"/>
       <c r="M18" s="15">
         <v>217</v>
       </c>
       <c r="N18" s="15" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="O18" s="14"/>
       <c r="P18" s="15">
         <v>267</v>
       </c>
       <c r="Q18" s="15" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="R18" s="14"/>
     </row>
@@ -3050,43 +3062,43 @@
       <c r="A19" s="15">
         <v>17</v>
       </c>
-      <c r="B19" s="15" t="s">
-        <v>189</v>
+      <c r="B19" s="16" t="s">
+        <v>188</v>
       </c>
       <c r="C19" s="14"/>
       <c r="D19" s="15">
         <v>68</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F19" s="14"/>
       <c r="G19" s="15">
         <v>118</v>
       </c>
       <c r="H19" s="15" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I19" s="14"/>
       <c r="J19" s="15">
         <v>168</v>
       </c>
       <c r="K19" s="15" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="L19" s="14"/>
       <c r="M19" s="15">
         <v>218</v>
       </c>
       <c r="N19" s="15" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="O19" s="14"/>
       <c r="P19" s="15">
         <v>268</v>
       </c>
       <c r="Q19" s="15" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="R19" s="14"/>
     </row>
@@ -3094,43 +3106,43 @@
       <c r="A20" s="15">
         <v>18</v>
       </c>
-      <c r="B20" s="15" t="s">
-        <v>195</v>
+      <c r="B20" s="16" t="s">
+        <v>194</v>
       </c>
       <c r="C20" s="14"/>
       <c r="D20" s="15">
         <v>69</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F20" s="14"/>
       <c r="G20" s="15">
         <v>119</v>
       </c>
       <c r="H20" s="15" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I20" s="14"/>
       <c r="J20" s="15">
         <v>169</v>
       </c>
       <c r="K20" s="15" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L20" s="14"/>
       <c r="M20" s="15">
         <v>219</v>
       </c>
       <c r="N20" s="15" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="O20" s="14"/>
       <c r="P20" s="15">
         <v>269</v>
       </c>
       <c r="Q20" s="15" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="R20" s="14"/>
     </row>
@@ -3138,43 +3150,43 @@
       <c r="A21" s="15">
         <v>19</v>
       </c>
-      <c r="B21" s="15" t="s">
-        <v>201</v>
+      <c r="B21" s="16" t="s">
+        <v>200</v>
       </c>
       <c r="C21" s="14"/>
       <c r="D21" s="15">
         <v>70</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F21" s="14"/>
       <c r="G21" s="15">
         <v>120</v>
       </c>
       <c r="H21" s="15" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I21" s="14"/>
       <c r="J21" s="15">
         <v>170</v>
       </c>
       <c r="K21" s="15" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="L21" s="14"/>
       <c r="M21" s="15">
         <v>220</v>
       </c>
       <c r="N21" s="15" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="O21" s="14"/>
       <c r="P21" s="15">
         <v>270</v>
       </c>
       <c r="Q21" s="15" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="R21" s="14"/>
     </row>
@@ -3182,43 +3194,43 @@
       <c r="A22" s="15">
         <v>20</v>
       </c>
-      <c r="B22" s="15" t="s">
-        <v>207</v>
+      <c r="B22" s="16" t="s">
+        <v>206</v>
       </c>
       <c r="C22" s="14"/>
       <c r="D22" s="15">
         <v>71</v>
       </c>
       <c r="E22" s="15" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F22" s="14"/>
       <c r="G22" s="15">
         <v>121</v>
       </c>
       <c r="H22" s="15" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I22" s="14"/>
       <c r="J22" s="15">
         <v>171</v>
       </c>
       <c r="K22" s="15" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="L22" s="14"/>
       <c r="M22" s="15">
         <v>221</v>
       </c>
       <c r="N22" s="15" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="O22" s="14"/>
       <c r="P22" s="15">
         <v>271</v>
       </c>
       <c r="Q22" s="15" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="R22" s="14"/>
     </row>
@@ -3227,42 +3239,42 @@
         <v>21</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C23" s="14"/>
       <c r="D23" s="15">
         <v>72</v>
       </c>
       <c r="E23" s="15" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F23" s="14"/>
       <c r="G23" s="15">
         <v>122</v>
       </c>
       <c r="H23" s="15" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I23" s="14"/>
       <c r="J23" s="15">
         <v>172</v>
       </c>
       <c r="K23" s="15" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="L23" s="14"/>
       <c r="M23" s="15">
         <v>222</v>
       </c>
       <c r="N23" s="15" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="O23" s="14"/>
       <c r="P23" s="15">
         <v>272</v>
       </c>
       <c r="Q23" s="15" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="R23" s="14"/>
     </row>
@@ -3271,42 +3283,42 @@
         <v>22</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C24" s="14"/>
       <c r="D24" s="15">
         <v>73</v>
       </c>
       <c r="E24" s="15" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F24" s="14"/>
       <c r="G24" s="15">
         <v>123</v>
       </c>
       <c r="H24" s="15" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I24" s="14"/>
       <c r="J24" s="15">
         <v>173</v>
       </c>
       <c r="K24" s="15" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="L24" s="14"/>
       <c r="M24" s="15">
         <v>223</v>
       </c>
       <c r="N24" s="15" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="O24" s="14"/>
       <c r="P24" s="15">
         <v>273</v>
       </c>
       <c r="Q24" s="15" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="R24" s="14"/>
     </row>
@@ -3315,42 +3327,42 @@
         <v>23</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C25" s="14"/>
       <c r="D25" s="15">
         <v>74</v>
       </c>
       <c r="E25" s="15" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F25" s="14"/>
       <c r="G25" s="15">
         <v>124</v>
       </c>
       <c r="H25" s="15" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I25" s="14"/>
       <c r="J25" s="15">
         <v>174</v>
       </c>
       <c r="K25" s="15" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="L25" s="14"/>
       <c r="M25" s="15">
         <v>224</v>
       </c>
       <c r="N25" s="15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="O25" s="14"/>
       <c r="P25" s="15">
         <v>274</v>
       </c>
       <c r="Q25" s="15" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="R25" s="14"/>
     </row>
@@ -3359,42 +3371,42 @@
         <v>24</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C26" s="14"/>
       <c r="D26" s="15">
         <v>75</v>
       </c>
       <c r="E26" s="15" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F26" s="14"/>
       <c r="G26" s="15">
         <v>125</v>
       </c>
       <c r="H26" s="15" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="I26" s="14"/>
       <c r="J26" s="15">
         <v>175</v>
       </c>
       <c r="K26" s="15" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="L26" s="14"/>
       <c r="M26" s="15">
         <v>225</v>
       </c>
       <c r="N26" s="15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="O26" s="14"/>
       <c r="P26" s="15">
         <v>275</v>
       </c>
       <c r="Q26" s="15" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="R26" s="14"/>
     </row>
@@ -3403,42 +3415,42 @@
         <v>25</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C27" s="14"/>
       <c r="D27" s="15">
         <v>76</v>
       </c>
       <c r="E27" s="15" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F27" s="14"/>
       <c r="G27" s="15">
         <v>126</v>
       </c>
       <c r="H27" s="15" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="I27" s="14"/>
       <c r="J27" s="15">
         <v>176</v>
       </c>
       <c r="K27" s="15" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="L27" s="14"/>
       <c r="M27" s="15">
         <v>226</v>
       </c>
       <c r="N27" s="15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="O27" s="14"/>
       <c r="P27" s="15">
         <v>276</v>
       </c>
       <c r="Q27" s="15" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="R27" s="14"/>
     </row>
@@ -3447,42 +3459,42 @@
         <v>26</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C28" s="14"/>
       <c r="D28" s="15">
         <v>77</v>
       </c>
       <c r="E28" s="15" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F28" s="14"/>
       <c r="G28" s="15">
         <v>127</v>
       </c>
       <c r="H28" s="15" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I28" s="14"/>
       <c r="J28" s="15">
         <v>177</v>
       </c>
       <c r="K28" s="15" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="L28" s="14"/>
       <c r="M28" s="15">
         <v>227</v>
       </c>
       <c r="N28" s="15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="O28" s="14"/>
       <c r="P28" s="15">
         <v>277</v>
       </c>
       <c r="Q28" s="15" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="R28" s="14"/>
     </row>
@@ -3491,42 +3503,42 @@
         <v>27</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C29" s="14"/>
       <c r="D29" s="15">
         <v>78</v>
       </c>
       <c r="E29" s="15" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F29" s="14"/>
       <c r="G29" s="15">
         <v>128</v>
       </c>
       <c r="H29" s="15" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="I29" s="14"/>
       <c r="J29" s="15">
         <v>178</v>
       </c>
       <c r="K29" s="15" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="L29" s="14"/>
       <c r="M29" s="15">
         <v>228</v>
       </c>
       <c r="N29" s="15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="O29" s="14"/>
       <c r="P29" s="15">
         <v>278</v>
       </c>
       <c r="Q29" s="15" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="R29" s="14"/>
     </row>
@@ -3535,42 +3547,42 @@
         <v>28</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C30" s="14"/>
       <c r="D30" s="15">
         <v>79</v>
       </c>
       <c r="E30" s="15" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F30" s="14"/>
       <c r="G30" s="15">
         <v>129</v>
       </c>
       <c r="H30" s="15" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I30" s="14"/>
       <c r="J30" s="15">
         <v>179</v>
       </c>
       <c r="K30" s="15" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="L30" s="14"/>
       <c r="M30" s="15">
         <v>229</v>
       </c>
       <c r="N30" s="15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="O30" s="14"/>
       <c r="P30" s="15">
         <v>279</v>
       </c>
       <c r="Q30" s="15" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="R30" s="14"/>
     </row>
@@ -3579,42 +3591,42 @@
         <v>29</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C31" s="14"/>
       <c r="D31" s="15">
         <v>80</v>
       </c>
       <c r="E31" s="15" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F31" s="14"/>
       <c r="G31" s="15">
         <v>130</v>
       </c>
       <c r="H31" s="15" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="I31" s="14"/>
       <c r="J31" s="15">
         <v>180</v>
       </c>
       <c r="K31" s="15" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="L31" s="14"/>
       <c r="M31" s="15">
         <v>230</v>
       </c>
       <c r="N31" s="15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="O31" s="14"/>
       <c r="P31" s="15">
         <v>280</v>
       </c>
       <c r="Q31" s="15" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="R31" s="14"/>
     </row>
@@ -3623,42 +3635,42 @@
         <v>30</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C32" s="14"/>
       <c r="D32" s="15">
         <v>81</v>
       </c>
       <c r="E32" s="15" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F32" s="14"/>
       <c r="G32" s="15">
         <v>131</v>
       </c>
       <c r="H32" s="15" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="I32" s="14"/>
       <c r="J32" s="15">
         <v>181</v>
       </c>
       <c r="K32" s="15" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="L32" s="14"/>
       <c r="M32" s="15">
         <v>231</v>
       </c>
       <c r="N32" s="15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="O32" s="14"/>
       <c r="P32" s="15">
         <v>281</v>
       </c>
       <c r="Q32" s="15" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="R32" s="14"/>
     </row>
@@ -3667,42 +3679,42 @@
         <v>31</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C33" s="14"/>
       <c r="D33" s="15">
         <v>82</v>
       </c>
       <c r="E33" s="15" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F33" s="14"/>
       <c r="G33" s="15">
         <v>132</v>
       </c>
       <c r="H33" s="15" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="I33" s="14"/>
       <c r="J33" s="15">
         <v>182</v>
       </c>
       <c r="K33" s="15" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="L33" s="14"/>
       <c r="M33" s="15">
         <v>232</v>
       </c>
       <c r="N33" s="15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="O33" s="14"/>
       <c r="P33" s="15">
         <v>282</v>
       </c>
       <c r="Q33" s="15" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="R33" s="14"/>
     </row>
@@ -3711,42 +3723,42 @@
         <v>32</v>
       </c>
       <c r="B34" s="15" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C34" s="14"/>
       <c r="D34" s="15">
         <v>83</v>
       </c>
       <c r="E34" s="15" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F34" s="14"/>
       <c r="G34" s="15">
         <v>133</v>
       </c>
       <c r="H34" s="15" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="I34" s="14"/>
       <c r="J34" s="15">
         <v>183</v>
       </c>
       <c r="K34" s="15" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="L34" s="14"/>
       <c r="M34" s="15">
         <v>233</v>
       </c>
       <c r="N34" s="15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="O34" s="14"/>
       <c r="P34" s="15">
         <v>283</v>
       </c>
       <c r="Q34" s="15" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="R34" s="14"/>
     </row>
@@ -3755,42 +3767,42 @@
         <v>33</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C35" s="14"/>
       <c r="D35" s="15">
         <v>84</v>
       </c>
       <c r="E35" s="15" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F35" s="14"/>
       <c r="G35" s="15">
         <v>134</v>
       </c>
       <c r="H35" s="15" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="I35" s="14"/>
       <c r="J35" s="15">
         <v>184</v>
       </c>
       <c r="K35" s="15" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="L35" s="14"/>
       <c r="M35" s="15">
         <v>234</v>
       </c>
       <c r="N35" s="15" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="O35" s="14"/>
       <c r="P35" s="15">
         <v>284</v>
       </c>
       <c r="Q35" s="15" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="R35" s="14"/>
     </row>
@@ -3799,42 +3811,42 @@
         <v>34</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C36" s="14"/>
       <c r="D36" s="15">
         <v>85</v>
       </c>
       <c r="E36" s="15" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F36" s="14"/>
       <c r="G36" s="15">
         <v>135</v>
       </c>
       <c r="H36" s="15" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="I36" s="14"/>
       <c r="J36" s="15">
         <v>185</v>
       </c>
       <c r="K36" s="15" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="L36" s="14"/>
       <c r="M36" s="15">
         <v>235</v>
       </c>
       <c r="N36" s="15" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="O36" s="14"/>
       <c r="P36" s="15">
         <v>285</v>
       </c>
       <c r="Q36" s="15" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="R36" s="14"/>
     </row>
@@ -3843,42 +3855,42 @@
         <v>35</v>
       </c>
       <c r="B37" s="15" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C37" s="14"/>
       <c r="D37" s="15">
         <v>86</v>
       </c>
       <c r="E37" s="15" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F37" s="14"/>
       <c r="G37" s="15">
         <v>136</v>
       </c>
       <c r="H37" s="15" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="I37" s="14"/>
       <c r="J37" s="15">
         <v>186</v>
       </c>
       <c r="K37" s="15" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="L37" s="14"/>
       <c r="M37" s="15">
         <v>236</v>
       </c>
       <c r="N37" s="15" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="O37" s="14"/>
       <c r="P37" s="15">
         <v>286</v>
       </c>
       <c r="Q37" s="15" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="R37" s="14"/>
     </row>
@@ -3887,42 +3899,42 @@
         <v>36</v>
       </c>
       <c r="B38" s="15" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C38" s="14"/>
       <c r="D38" s="15">
         <v>87</v>
       </c>
       <c r="E38" s="15" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F38" s="14"/>
       <c r="G38" s="15">
         <v>137</v>
       </c>
       <c r="H38" s="15" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I38" s="14"/>
       <c r="J38" s="15">
         <v>187</v>
       </c>
       <c r="K38" s="15" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="L38" s="14"/>
       <c r="M38" s="15">
         <v>237</v>
       </c>
       <c r="N38" s="15" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="O38" s="14"/>
       <c r="P38" s="15">
         <v>287</v>
       </c>
       <c r="Q38" s="15" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="R38" s="14"/>
     </row>
@@ -3931,42 +3943,42 @@
         <v>37</v>
       </c>
       <c r="B39" s="15" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C39" s="14"/>
       <c r="D39" s="15">
         <v>88</v>
       </c>
       <c r="E39" s="15" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F39" s="14"/>
       <c r="G39" s="15">
         <v>138</v>
       </c>
       <c r="H39" s="15" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="I39" s="14"/>
       <c r="J39" s="15">
         <v>188</v>
       </c>
       <c r="K39" s="15" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="L39" s="14"/>
       <c r="M39" s="15">
         <v>238</v>
       </c>
       <c r="N39" s="15" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="O39" s="14"/>
       <c r="P39" s="15">
         <v>288</v>
       </c>
       <c r="Q39" s="15" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="R39" s="14"/>
     </row>
@@ -3975,42 +3987,42 @@
         <v>38</v>
       </c>
       <c r="B40" s="15" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C40" s="14"/>
       <c r="D40" s="15">
         <v>89</v>
       </c>
       <c r="E40" s="15" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F40" s="14"/>
       <c r="G40" s="15">
         <v>139</v>
       </c>
       <c r="H40" s="15" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="I40" s="14"/>
       <c r="J40" s="15">
         <v>189</v>
       </c>
       <c r="K40" s="15" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="L40" s="14"/>
       <c r="M40" s="15">
         <v>239</v>
       </c>
       <c r="N40" s="15" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="O40" s="14"/>
       <c r="P40" s="15">
         <v>289</v>
       </c>
       <c r="Q40" s="15" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="R40" s="14"/>
     </row>
@@ -4019,42 +4031,42 @@
         <v>39</v>
       </c>
       <c r="B41" s="15" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C41" s="14"/>
       <c r="D41" s="15">
         <v>90</v>
       </c>
       <c r="E41" s="15" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F41" s="14"/>
       <c r="G41" s="15">
         <v>140</v>
       </c>
       <c r="H41" s="15" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="I41" s="14"/>
       <c r="J41" s="15">
         <v>190</v>
       </c>
       <c r="K41" s="15" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="L41" s="14"/>
       <c r="M41" s="15">
         <v>240</v>
       </c>
       <c r="N41" s="15" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="O41" s="14"/>
       <c r="P41" s="15">
         <v>290</v>
       </c>
       <c r="Q41" s="15" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="R41" s="14"/>
     </row>
@@ -4063,42 +4075,42 @@
         <v>40</v>
       </c>
       <c r="B42" s="15" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C42" s="14"/>
       <c r="D42" s="15">
         <v>91</v>
       </c>
       <c r="E42" s="15" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F42" s="14"/>
       <c r="G42" s="15">
         <v>141</v>
       </c>
       <c r="H42" s="15" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="I42" s="14"/>
       <c r="J42" s="15">
         <v>191</v>
       </c>
       <c r="K42" s="15" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="L42" s="14"/>
       <c r="M42" s="15">
         <v>241</v>
       </c>
       <c r="N42" s="15" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="O42" s="14"/>
       <c r="P42" s="15">
         <v>291</v>
       </c>
       <c r="Q42" s="15" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="R42" s="14"/>
     </row>
@@ -4107,42 +4119,42 @@
         <v>41</v>
       </c>
       <c r="B43" s="15" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C43" s="14"/>
       <c r="D43" s="15">
         <v>92</v>
       </c>
       <c r="E43" s="15" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="F43" s="14"/>
       <c r="G43" s="15">
         <v>142</v>
       </c>
       <c r="H43" s="15" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="I43" s="14"/>
       <c r="J43" s="15">
         <v>192</v>
       </c>
       <c r="K43" s="15" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="L43" s="14"/>
       <c r="M43" s="15">
         <v>242</v>
       </c>
       <c r="N43" s="15" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="O43" s="14"/>
       <c r="P43" s="15">
         <v>292</v>
       </c>
       <c r="Q43" s="15" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="R43" s="14"/>
     </row>
@@ -4151,42 +4163,42 @@
         <v>42</v>
       </c>
       <c r="B44" s="15" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C44" s="14"/>
       <c r="D44" s="15">
         <v>93</v>
       </c>
       <c r="E44" s="15" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F44" s="14"/>
       <c r="G44" s="15">
         <v>143</v>
       </c>
       <c r="H44" s="15" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="I44" s="14"/>
       <c r="J44" s="15">
         <v>193</v>
       </c>
       <c r="K44" s="15" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="L44" s="14"/>
       <c r="M44" s="15">
         <v>243</v>
       </c>
       <c r="N44" s="15" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="O44" s="14"/>
       <c r="P44" s="15">
         <v>293</v>
       </c>
       <c r="Q44" s="15" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="R44" s="14"/>
     </row>
@@ -4195,42 +4207,42 @@
         <v>43</v>
       </c>
       <c r="B45" s="15" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C45" s="14"/>
       <c r="D45" s="15">
         <v>94</v>
       </c>
       <c r="E45" s="15" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="F45" s="14"/>
       <c r="G45" s="15">
         <v>144</v>
       </c>
       <c r="H45" s="15" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="I45" s="14"/>
       <c r="J45" s="15">
         <v>194</v>
       </c>
       <c r="K45" s="15" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="L45" s="14"/>
       <c r="M45" s="15">
         <v>244</v>
       </c>
       <c r="N45" s="15" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="O45" s="14"/>
       <c r="P45" s="15">
         <v>294</v>
       </c>
       <c r="Q45" s="15" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="R45" s="14"/>
     </row>
@@ -4239,42 +4251,42 @@
         <v>44</v>
       </c>
       <c r="B46" s="15" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C46" s="14"/>
       <c r="D46" s="15">
         <v>95</v>
       </c>
       <c r="E46" s="15" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="F46" s="14"/>
       <c r="G46" s="15">
         <v>145</v>
       </c>
       <c r="H46" s="15" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="I46" s="14"/>
       <c r="J46" s="15">
         <v>195</v>
       </c>
       <c r="K46" s="15" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="L46" s="14"/>
       <c r="M46" s="15">
         <v>245</v>
       </c>
       <c r="N46" s="15" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="O46" s="14"/>
       <c r="P46" s="15">
         <v>295</v>
       </c>
       <c r="Q46" s="15" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="R46" s="14"/>
     </row>
@@ -4283,42 +4295,42 @@
         <v>45</v>
       </c>
       <c r="B47" s="15" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C47" s="14"/>
       <c r="D47" s="15">
         <v>96</v>
       </c>
       <c r="E47" s="15" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="F47" s="14"/>
       <c r="G47" s="15">
         <v>146</v>
       </c>
       <c r="H47" s="15" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I47" s="14"/>
       <c r="J47" s="15">
         <v>196</v>
       </c>
       <c r="K47" s="15" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="L47" s="14"/>
       <c r="M47" s="15">
         <v>246</v>
       </c>
       <c r="N47" s="15" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="O47" s="14"/>
       <c r="P47" s="15">
         <v>296</v>
       </c>
       <c r="Q47" s="15" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="R47" s="14"/>
     </row>
@@ -4327,42 +4339,42 @@
         <v>46</v>
       </c>
       <c r="B48" s="15" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C48" s="14"/>
       <c r="D48" s="15">
         <v>97</v>
       </c>
       <c r="E48" s="15" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="F48" s="14"/>
       <c r="G48" s="15">
         <v>147</v>
       </c>
       <c r="H48" s="15" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="I48" s="14"/>
       <c r="J48" s="15">
         <v>197</v>
       </c>
       <c r="K48" s="15" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="L48" s="14"/>
       <c r="M48" s="15">
         <v>247</v>
       </c>
       <c r="N48" s="15" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="O48" s="14"/>
       <c r="P48" s="15">
         <v>297</v>
       </c>
       <c r="Q48" s="15" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="R48" s="14"/>
     </row>
@@ -4371,42 +4383,42 @@
         <v>47</v>
       </c>
       <c r="B49" s="15" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C49" s="14"/>
       <c r="D49" s="15">
         <v>98</v>
       </c>
       <c r="E49" s="15" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="F49" s="14"/>
       <c r="G49" s="15">
         <v>148</v>
       </c>
       <c r="H49" s="15" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="I49" s="14"/>
       <c r="J49" s="15">
         <v>198</v>
       </c>
       <c r="K49" s="15" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="L49" s="14"/>
       <c r="M49" s="15">
         <v>248</v>
       </c>
       <c r="N49" s="15" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="O49" s="14"/>
       <c r="P49" s="15">
         <v>298</v>
       </c>
       <c r="Q49" s="15" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="R49" s="14"/>
     </row>
@@ -4415,42 +4427,42 @@
         <v>48</v>
       </c>
       <c r="B50" s="15" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C50" s="14"/>
       <c r="D50" s="15">
         <v>99</v>
       </c>
       <c r="E50" s="15" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="F50" s="14"/>
       <c r="G50" s="15">
         <v>149</v>
       </c>
       <c r="H50" s="15" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="I50" s="14"/>
       <c r="J50" s="15">
         <v>199</v>
       </c>
       <c r="K50" s="15" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="L50" s="14"/>
       <c r="M50" s="15">
         <v>249</v>
       </c>
       <c r="N50" s="15" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="O50" s="14"/>
       <c r="P50" s="15">
         <v>299</v>
       </c>
       <c r="Q50" s="15" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="R50" s="14"/>
     </row>
@@ -4459,42 +4471,42 @@
         <v>49</v>
       </c>
       <c r="B51" s="15" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C51" s="14"/>
       <c r="D51" s="15">
         <v>100</v>
       </c>
       <c r="E51" s="15" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="F51" s="14"/>
       <c r="G51" s="15">
         <v>150</v>
       </c>
       <c r="H51" s="15" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="I51" s="14"/>
       <c r="J51" s="15">
         <v>200</v>
       </c>
       <c r="K51" s="15" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="L51" s="14"/>
       <c r="M51" s="15">
         <v>250</v>
       </c>
       <c r="N51" s="15" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="O51" s="14"/>
       <c r="P51" s="15">
         <v>300</v>
       </c>
       <c r="Q51" s="15" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="R51" s="14"/>
     </row>
@@ -4503,7 +4515,7 @@
         <v>50</v>
       </c>
       <c r="B52" s="15" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C52" s="14"/>
       <c r="D52" s="15"/>
@@ -4570,49 +4582,53 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCCF9E71-D3B5-42A3-9DB3-24557FECF4AE}">
-  <dimension ref="A1:G500"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{404C34B9-A0ED-4FA3-AC84-23555E254077}">
+  <dimension ref="A1:H500"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.42578125" style="4"/>
     <col min="2" max="2" width="17.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="29.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="43" style="1" customWidth="1"/>
-    <col min="6" max="6" width="62.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="72.7109375" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="14.42578125" style="1"/>
+    <col min="3" max="3" width="35" style="1" customWidth="1"/>
+    <col min="4" max="4" width="29.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="43" style="1" customWidth="1"/>
+    <col min="7" max="7" width="62.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="72.7109375" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="14.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>2</v>
+        <v>399</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>76</v>
+        <v>398</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -4620,20 +4636,20 @@
         <f>"CHAT" &amp; TEXT(DEC2HEX(A2, 5), "00000")</f>
         <v>CHAT00001</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="D2" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -4641,20 +4657,20 @@
         <f t="shared" ref="B3:B66" si="0">"CHAT" &amp; TEXT(DEC2HEX(A3, 5), "00000")</f>
         <v>CHAT00002</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="D3" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>381</v>
+        <v>76</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>380</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -4662,20 +4678,20 @@
         <f t="shared" si="0"/>
         <v>CHAT00003</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="D4" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -4683,20 +4699,20 @@
         <f t="shared" si="0"/>
         <v>CHAT00004</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="D5" s="1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>381</v>
+        <v>78</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>380</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -4704,21 +4720,22 @@
         <f t="shared" si="0"/>
         <v>CHAT00005</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D6" s="17" t="s">
-        <v>80</v>
+      <c r="C6" s="17"/>
+      <c r="D6" s="1" t="s">
+        <v>74</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>381</v>
+        <v>79</v>
       </c>
       <c r="F6" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="G6" s="17"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>380</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="H6" s="17"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -4727,7 +4744,7 @@
         <v>CHAT00006</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -4735,23 +4752,24 @@
         <f t="shared" si="0"/>
         <v>CHAT00007</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="17"/>
+      <c r="D8" s="17" t="s">
+        <v>377</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>385</v>
+      </c>
+      <c r="G8" s="17" t="s">
         <v>378</v>
       </c>
-      <c r="D8" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="E8" s="17" t="s">
-        <v>386</v>
-      </c>
-      <c r="F8" s="17" t="s">
-        <v>379</v>
-      </c>
-      <c r="G8" s="17" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8" s="17" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -4759,20 +4777,21 @@
         <f t="shared" si="0"/>
         <v>CHAT00008</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E9" s="19" t="s">
-        <v>382</v>
+      <c r="C9" s="20"/>
+      <c r="E9" s="1" t="s">
+        <v>76</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>380</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>381</v>
+      </c>
+      <c r="G9" s="19" t="s">
+        <v>379</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -4780,17 +4799,17 @@
         <f t="shared" si="0"/>
         <v>CHAT00009</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>78</v>
-      </c>
       <c r="E10" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -4798,17 +4817,17 @@
         <f t="shared" si="0"/>
         <v>CHAT0000A</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>78</v>
-      </c>
       <c r="E11" s="1" t="s">
-        <v>389</v>
+        <v>77</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>388</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -4816,17 +4835,17 @@
         <f t="shared" si="0"/>
         <v>CHAT0000B</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>78</v>
-      </c>
       <c r="E12" s="1" t="s">
-        <v>391</v>
+        <v>77</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>390</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -4834,17 +4853,17 @@
         <f t="shared" si="0"/>
         <v>CHAT0000C</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>78</v>
-      </c>
       <c r="E13" s="1" t="s">
-        <v>390</v>
+        <v>77</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>389</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -4852,17 +4871,17 @@
         <f t="shared" si="0"/>
         <v>CHAT0000D</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>78</v>
-      </c>
       <c r="E14" s="1" t="s">
-        <v>392</v>
+        <v>77</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>391</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -4870,17 +4889,17 @@
         <f t="shared" si="0"/>
         <v>CHAT0000E</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>78</v>
-      </c>
       <c r="E15" s="1" t="s">
-        <v>393</v>
+        <v>77</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>392</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -8952,7 +8971,7 @@
       <c r="B500" s="5"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C17:G23">
+  <conditionalFormatting sqref="C17:H23">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"N"</formula>
     </cfRule>
@@ -8966,6 +8985,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A855378936633F46935DE081F3F0A723" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6fb8377a16f57469f31fda63402737be">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="0e1bb11d-1fe8-4e80-a80d-c671e8cd2a50" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a5a807ddb17e97ebd5eac858e2e697fd" ns3:_="">
     <xsd:import namespace="0e1bb11d-1fe8-4e80-a80d-c671e8cd2a50"/>
@@ -9167,22 +9201,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{88BC72A4-2999-4A2E-B325-3F14F9A9DFDC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="0e1bb11d-1fe8-4e80-a80d-c671e8cd2a50"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DF4A1F3-27F5-4026-9F7B-EA2EEA754838}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8A8016DE-DC46-404F-9AC8-AB31FBBA1BB2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9198,28 +9241,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DF4A1F3-27F5-4026-9F7B-EA2EEA754838}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{88BC72A4-2999-4A2E-B325-3F14F9A9DFDC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="0e1bb11d-1fe8-4e80-a80d-c671e8cd2a50"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Working on Correcting Minor issues
</commit_message>
<xml_diff>
--- a/FullStackProject/documentation/serverAPIs.xlsx
+++ b/FullStackProject/documentation/serverAPIs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Html_CSS\FullStackProject\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67345C84-F110-4B00-8D12-91EFD0C213AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA3B445D-94FD-49CE-97C9-104455B1B2C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4605" yWindow="3315" windowWidth="21600" windowHeight="11835" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Error Code" sheetId="17" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="394">
   <si>
     <t xml:space="preserve">Sr </t>
   </si>
@@ -1174,18 +1174,12 @@
     <t>Chat Management</t>
   </si>
   <si>
-    <t>Give List of different chats that a user has</t>
-  </si>
-  <si>
     <t>Give list of all msg that chat has with userId</t>
   </si>
   <si>
     <t>/users/{userId}</t>
   </si>
   <si>
-    <t>/chat/{userId}</t>
-  </si>
-  <si>
     <t>Extra</t>
   </si>
   <si>
@@ -1195,49 +1189,37 @@
     <t>chats represent conversiation with other users in privately or group</t>
   </si>
   <si>
-    <t>/chatlist</t>
-  </si>
-  <si>
-    <t>/chat/text</t>
-  </si>
-  <si>
-    <t>Add text msg to the chat &amp; text table</t>
-  </si>
-  <si>
-    <t>/chat/file</t>
-  </si>
-  <si>
-    <t>/chat/payment</t>
-  </si>
-  <si>
-    <t>/chat/meeting</t>
-  </si>
-  <si>
-    <t>/chat/callUp</t>
-  </si>
-  <si>
-    <t>/chat/location</t>
-  </si>
-  <si>
-    <t>Add file to the chat &amp; file table</t>
-  </si>
-  <si>
-    <t>Add meeting to the chat &amp; meeting table</t>
-  </si>
-  <si>
-    <t>Add location to the chat &amp; location table</t>
-  </si>
-  <si>
-    <t>Add callup to the chat &amp; callUp table</t>
-  </si>
-  <si>
-    <t>Add payment to the chat &amp; payment table</t>
-  </si>
-  <si>
     <t>Folder Name</t>
   </si>
   <si>
     <t>Response Codes</t>
+  </si>
+  <si>
+    <t>/getChatList</t>
+  </si>
+  <si>
+    <t>Add Any kind of  msg to the message &amp; respective table</t>
+  </si>
+  <si>
+    <t>/createChat</t>
+  </si>
+  <si>
+    <t>To Create Private Chat</t>
+  </si>
+  <si>
+    <t>/createGroupChat</t>
+  </si>
+  <si>
+    <t>To Create group Chat</t>
+  </si>
+  <si>
+    <t>To get the List of private &amp; group chats</t>
+  </si>
+  <si>
+    <t>/getChat/:chatId</t>
+  </si>
+  <si>
+    <t>/addMsg/:chatId</t>
   </si>
 </sst>
 </file>
@@ -1828,7 +1810,7 @@
   <dimension ref="A1:D40"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="17.45" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2245,8 +2227,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8787874B-90D5-45F1-9880-0373B280E830}">
   <dimension ref="A1:R52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3238,7 +3220,7 @@
       <c r="A23" s="15">
         <v>21</v>
       </c>
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="16" t="s">
         <v>212</v>
       </c>
       <c r="C23" s="14"/>
@@ -3282,7 +3264,7 @@
       <c r="A24" s="15">
         <v>22</v>
       </c>
-      <c r="B24" s="15" t="s">
+      <c r="B24" s="16" t="s">
         <v>218</v>
       </c>
       <c r="C24" s="14"/>
@@ -3326,7 +3308,7 @@
       <c r="A25" s="15">
         <v>23</v>
       </c>
-      <c r="B25" s="15" t="s">
+      <c r="B25" s="16" t="s">
         <v>224</v>
       </c>
       <c r="C25" s="14"/>
@@ -3370,7 +3352,7 @@
       <c r="A26" s="15">
         <v>24</v>
       </c>
-      <c r="B26" s="15" t="s">
+      <c r="B26" s="16" t="s">
         <v>229</v>
       </c>
       <c r="C26" s="14"/>
@@ -3414,7 +3396,7 @@
       <c r="A27" s="15">
         <v>25</v>
       </c>
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="16" t="s">
         <v>234</v>
       </c>
       <c r="C27" s="14"/>
@@ -4585,8 +4567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{404C34B9-A0ED-4FA3-AC84-23555E254077}">
   <dimension ref="A1:H500"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4610,10 +4592,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>399</v>
+        <v>384</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>398</v>
+        <v>383</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>75</v>
@@ -4625,7 +4607,7 @@
         <v>72</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -4664,7 +4646,7 @@
         <v>76</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>82</v>
@@ -4706,7 +4688,7 @@
         <v>78</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>84</v>
@@ -4728,7 +4710,7 @@
         <v>79</v>
       </c>
       <c r="F6" s="17" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="G6" s="17" t="s">
         <v>85</v>
@@ -4757,16 +4739,16 @@
         <v>377</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F8" s="17" t="s">
         <v>385</v>
       </c>
       <c r="G8" s="17" t="s">
-        <v>378</v>
+        <v>391</v>
       </c>
       <c r="H8" s="17" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -4782,13 +4764,13 @@
         <v>76</v>
       </c>
       <c r="F9" s="19" t="s">
+        <v>392</v>
+      </c>
+      <c r="G9" s="19" t="s">
+        <v>378</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>381</v>
-      </c>
-      <c r="G9" s="19" t="s">
-        <v>379</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -4803,10 +4785,10 @@
         <v>77</v>
       </c>
       <c r="F10" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>386</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -4821,10 +4803,10 @@
         <v>77</v>
       </c>
       <c r="F11" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>388</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -4839,10 +4821,10 @@
         <v>77</v>
       </c>
       <c r="F12" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>390</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -4853,15 +4835,6 @@
         <f t="shared" si="0"/>
         <v>CHAT0000C</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>389</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>397</v>
-      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
@@ -4871,15 +4844,6 @@
         <f t="shared" si="0"/>
         <v>CHAT0000D</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>391</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>396</v>
-      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
@@ -4888,15 +4852,6 @@
       <c r="B15" s="5" t="str">
         <f t="shared" si="0"/>
         <v>CHAT0000E</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>392</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Good : text & Payment Handle
</commit_message>
<xml_diff>
--- a/FullStackProject/documentation/serverAPIs.xlsx
+++ b/FullStackProject/documentation/serverAPIs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Html_CSS\FullStackProject\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA3B445D-94FD-49CE-97C9-104455B1B2C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91D0B80B-05E2-465C-B527-96C0BE348A03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4605" yWindow="3315" windowWidth="21600" windowHeight="11835" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Error Code" sheetId="17" r:id="rId1"/>
@@ -1216,10 +1216,10 @@
     <t>To get the List of private &amp; group chats</t>
   </si>
   <si>
-    <t>/getChat/:chatId</t>
-  </si>
-  <si>
-    <t>/addMsg/:chatId</t>
+    <t>/addMsg/</t>
+  </si>
+  <si>
+    <t>/getChat/</t>
   </si>
 </sst>
 </file>
@@ -2228,7 +2228,7 @@
   <dimension ref="A1:R52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3440,7 +3440,7 @@
       <c r="A28" s="15">
         <v>26</v>
       </c>
-      <c r="B28" s="15" t="s">
+      <c r="B28" s="16" t="s">
         <v>239</v>
       </c>
       <c r="C28" s="14"/>
@@ -3484,7 +3484,7 @@
       <c r="A29" s="15">
         <v>27</v>
       </c>
-      <c r="B29" s="15" t="s">
+      <c r="B29" s="16" t="s">
         <v>244</v>
       </c>
       <c r="C29" s="14"/>
@@ -3528,7 +3528,7 @@
       <c r="A30" s="15">
         <v>28</v>
       </c>
-      <c r="B30" s="15" t="s">
+      <c r="B30" s="16" t="s">
         <v>249</v>
       </c>
       <c r="C30" s="14"/>
@@ -3572,7 +3572,7 @@
       <c r="A31" s="15">
         <v>29</v>
       </c>
-      <c r="B31" s="15" t="s">
+      <c r="B31" s="16" t="s">
         <v>254</v>
       </c>
       <c r="C31" s="14"/>
@@ -3616,7 +3616,7 @@
       <c r="A32" s="15">
         <v>30</v>
       </c>
-      <c r="B32" s="15" t="s">
+      <c r="B32" s="16" t="s">
         <v>259</v>
       </c>
       <c r="C32" s="14"/>
@@ -3660,7 +3660,7 @@
       <c r="A33" s="15">
         <v>31</v>
       </c>
-      <c r="B33" s="15" t="s">
+      <c r="B33" s="16" t="s">
         <v>264</v>
       </c>
       <c r="C33" s="14"/>
@@ -3704,7 +3704,7 @@
       <c r="A34" s="15">
         <v>32</v>
       </c>
-      <c r="B34" s="15" t="s">
+      <c r="B34" s="16" t="s">
         <v>269</v>
       </c>
       <c r="C34" s="14"/>
@@ -4568,7 +4568,7 @@
   <dimension ref="A1:H500"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4764,7 +4764,7 @@
         <v>76</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="G9" s="19" t="s">
         <v>378</v>
@@ -4785,7 +4785,7 @@
         <v>77</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>386</v>
@@ -8940,21 +8940,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A855378936633F46935DE081F3F0A723" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6fb8377a16f57469f31fda63402737be">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="0e1bb11d-1fe8-4e80-a80d-c671e8cd2a50" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a5a807ddb17e97ebd5eac858e2e697fd" ns3:_="">
     <xsd:import namespace="0e1bb11d-1fe8-4e80-a80d-c671e8cd2a50"/>
@@ -9156,31 +9141,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{88BC72A4-2999-4A2E-B325-3F14F9A9DFDC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="0e1bb11d-1fe8-4e80-a80d-c671e8cd2a50"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DF4A1F3-27F5-4026-9F7B-EA2EEA754838}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8A8016DE-DC46-404F-9AC8-AB31FBBA1BB2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9196,4 +9172,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DF4A1F3-27F5-4026-9F7B-EA2EEA754838}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{88BC72A4-2999-4A2E-B325-3F14F9A9DFDC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="0e1bb11d-1fe8-4e80-a80d-c671e8cd2a50"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add : verifyUser & API update
</commit_message>
<xml_diff>
--- a/FullStackProject/documentation/serverAPIs.xlsx
+++ b/FullStackProject/documentation/serverAPIs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Html_CSS\FullStackProject\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91D0B80B-05E2-465C-B527-96C0BE348A03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDDD5684-E937-4404-80DB-E5CBCAEEC320}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Error Code" sheetId="17" r:id="rId1"/>
@@ -2227,7 +2227,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8787874B-90D5-45F1-9880-0373B280E830}">
   <dimension ref="A1:R52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
@@ -3748,7 +3748,7 @@
       <c r="A35" s="15">
         <v>33</v>
       </c>
-      <c r="B35" s="15" t="s">
+      <c r="B35" s="16" t="s">
         <v>274</v>
       </c>
       <c r="C35" s="14"/>
@@ -3792,7 +3792,7 @@
       <c r="A36" s="15">
         <v>34</v>
       </c>
-      <c r="B36" s="15" t="s">
+      <c r="B36" s="16" t="s">
         <v>280</v>
       </c>
       <c r="C36" s="14"/>
@@ -3836,7 +3836,7 @@
       <c r="A37" s="15">
         <v>35</v>
       </c>
-      <c r="B37" s="15" t="s">
+      <c r="B37" s="16" t="s">
         <v>286</v>
       </c>
       <c r="C37" s="14"/>
@@ -4567,7 +4567,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{404C34B9-A0ED-4FA3-AC84-23555E254077}">
   <dimension ref="A1:H500"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update: its Working Good till this point
</commit_message>
<xml_diff>
--- a/FullStackProject/documentation/serverAPIs.xlsx
+++ b/FullStackProject/documentation/serverAPIs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Html_CSS\FullStackProject\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDDD5684-E937-4404-80DB-E5CBCAEEC320}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1100B928-BED9-4D23-9425-8BDA622C950E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2228,7 +2228,7 @@
   <dimension ref="A1:R52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3880,7 +3880,7 @@
       <c r="A38" s="15">
         <v>36</v>
       </c>
-      <c r="B38" s="15" t="s">
+      <c r="B38" s="16" t="s">
         <v>292</v>
       </c>
       <c r="C38" s="14"/>
@@ -8940,6 +8940,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A855378936633F46935DE081F3F0A723" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6fb8377a16f57469f31fda63402737be">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="0e1bb11d-1fe8-4e80-a80d-c671e8cd2a50" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a5a807ddb17e97ebd5eac858e2e697fd" ns3:_="">
     <xsd:import namespace="0e1bb11d-1fe8-4e80-a80d-c671e8cd2a50"/>
@@ -9141,22 +9156,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{88BC72A4-2999-4A2E-B325-3F14F9A9DFDC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="0e1bb11d-1fe8-4e80-a80d-c671e8cd2a50"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DF4A1F3-27F5-4026-9F7B-EA2EEA754838}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8A8016DE-DC46-404F-9AC8-AB31FBBA1BB2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9172,28 +9196,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DF4A1F3-27F5-4026-9F7B-EA2EEA754838}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{88BC72A4-2999-4A2E-B325-3F14F9A9DFDC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="0e1bb11d-1fe8-4e80-a80d-c671e8cd2a50"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>